<commit_message>
More appropriate fix for using strings in linked_table
</commit_message>
<xml_diff>
--- a/app/config/tables/Ethiopia_household/forms/Ethiopia_household/Ethiopia_household.xlsx
+++ b/app/config/tables/Ethiopia_household/forms/Ethiopia_household/Ethiopia_household.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\toolsuite\app-designer\app\config\tables\Ethiopia_household\forms\Ethiopia_household\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="65" yWindow="0" windowWidth="30737" windowHeight="16665" tabRatio="500" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="60" yWindow="0" windowWidth="30740" windowHeight="16660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="queries" sheetId="9" r:id="rId1"/>
@@ -987,7 +982,7 @@
     <t>filters by both the household_id and the age</t>
   </si>
   <si>
-    <t>'household_id='+encodeURIComponent(data('household_id'))</t>
+    <t>'household_id='+opendatakit.encodeURIDataElement('household_id')</t>
   </si>
 </sst>
 </file>
@@ -1946,23 +1941,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q25"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" topLeftCell="C8" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" customWidth="1"/>
+    <col min="1" max="1" width="19.83203125" customWidth="1"/>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" customWidth="1"/>
-    <col min="4" max="4" width="26.77734375" customWidth="1"/>
-    <col min="5" max="5" width="20.44140625" customWidth="1"/>
+    <col min="4" max="4" width="26.83203125" customWidth="1"/>
+    <col min="5" max="5" width="20.5" customWidth="1"/>
     <col min="6" max="6" width="23.33203125" customWidth="1"/>
-    <col min="7" max="7" width="26.109375" customWidth="1"/>
+    <col min="7" max="7" width="26.1640625" customWidth="1"/>
     <col min="8" max="8" width="39.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="46" customFormat="1">
       <c r="A1" s="44" t="s">
         <v>77</v>
       </c>
@@ -1988,7 +1983,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1">
       <c r="A2" s="36" t="s">
         <v>306</v>
       </c>
@@ -2000,7 +1995,7 @@
       <c r="G2" s="34"/>
       <c r="H2" s="34"/>
     </row>
-    <row r="3" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1">
       <c r="A3" s="36" t="s">
         <v>307</v>
       </c>
@@ -2012,7 +2007,7 @@
       <c r="G3" s="34"/>
       <c r="H3" s="34"/>
     </row>
-    <row r="4" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1">
       <c r="A4" s="36" t="s">
         <v>308</v>
       </c>
@@ -2024,7 +2019,7 @@
       <c r="G4" s="34"/>
       <c r="H4" s="34"/>
     </row>
-    <row r="5" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1">
       <c r="A5" s="36" t="s">
         <v>309</v>
       </c>
@@ -2036,7 +2031,7 @@
       <c r="G5" s="34"/>
       <c r="H5" s="34"/>
     </row>
-    <row r="6" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1">
       <c r="A6" s="36" t="s">
         <v>310</v>
       </c>
@@ -2048,7 +2043,7 @@
       <c r="G6" s="34"/>
       <c r="H6" s="34"/>
     </row>
-    <row r="7" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1">
       <c r="A7" s="36" t="s">
         <v>311</v>
       </c>
@@ -2060,7 +2055,7 @@
       <c r="G7" s="34"/>
       <c r="H7" s="34"/>
     </row>
-    <row r="8" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1">
       <c r="A8" s="36"/>
       <c r="B8" s="33"/>
       <c r="C8" s="33"/>
@@ -2070,7 +2065,7 @@
       <c r="G8" s="34"/>
       <c r="H8" s="34"/>
     </row>
-    <row r="9" spans="1:17" ht="47.15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="45">
       <c r="A9" s="3" t="s">
         <v>305</v>
       </c>
@@ -2096,7 +2091,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="30">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
         <v>107</v>
@@ -2120,7 +2115,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" ht="30">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
         <v>108</v>
@@ -2144,7 +2139,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="12" customFormat="1" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" s="12" customFormat="1" ht="30" customHeight="1">
       <c r="A12" s="12" t="s">
         <v>316</v>
       </c>
@@ -2175,7 +2170,7 @@
       <c r="P12" s="11"/>
       <c r="Q12" s="11"/>
     </row>
-    <row r="13" spans="1:17" s="1" customFormat="1" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="B13" s="3" t="s">
         <v>133</v>
       </c>
@@ -2203,7 +2198,7 @@
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
     </row>
-    <row r="14" spans="1:17" s="1" customFormat="1" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="B14" s="3" t="s">
         <v>134</v>
       </c>
@@ -2231,7 +2226,7 @@
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
     </row>
-    <row r="15" spans="1:17" s="1" customFormat="1" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="B15" s="3" t="s">
         <v>141</v>
       </c>
@@ -2259,7 +2254,7 @@
       <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
     </row>
-    <row r="16" spans="1:17" s="1" customFormat="1" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="B16" s="3" t="s">
         <v>153</v>
       </c>
@@ -2287,7 +2282,7 @@
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
     </row>
-    <row r="17" spans="1:17" s="1" customFormat="1" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="B17" s="3" t="s">
         <v>158</v>
       </c>
@@ -2315,7 +2310,7 @@
       <c r="P17" s="3"/>
       <c r="Q17" s="3"/>
     </row>
-    <row r="18" spans="1:17" s="1" customFormat="1" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="B18" s="3" t="s">
         <v>163</v>
       </c>
@@ -2343,7 +2338,7 @@
       <c r="P18" s="3"/>
       <c r="Q18" s="3"/>
     </row>
-    <row r="19" spans="1:17" s="1" customFormat="1" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="B19" s="3" t="s">
         <v>167</v>
       </c>
@@ -2371,7 +2366,7 @@
       <c r="P19" s="3"/>
       <c r="Q19" s="3"/>
     </row>
-    <row r="20" spans="1:17" s="1" customFormat="1" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="B20" s="3" t="s">
         <v>214</v>
       </c>
@@ -2399,7 +2394,7 @@
       <c r="P20" s="3"/>
       <c r="Q20" s="3"/>
     </row>
-    <row r="21" spans="1:17" s="1" customFormat="1" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="B21" s="3" t="s">
         <v>242</v>
       </c>
@@ -2427,7 +2422,7 @@
       <c r="P21" s="3"/>
       <c r="Q21" s="3"/>
     </row>
-    <row r="22" spans="1:17" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" ht="30">
       <c r="A22" s="3"/>
       <c r="B22" s="3" t="s">
         <v>286</v>
@@ -2451,7 +2446,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" ht="30">
       <c r="A23" s="3"/>
       <c r="B23" s="3" t="s">
         <v>287</v>
@@ -2475,7 +2470,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" ht="30">
       <c r="A24" s="3"/>
       <c r="B24" s="3" t="s">
         <v>291</v>
@@ -2499,7 +2494,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" ht="30">
       <c r="A25" s="3"/>
       <c r="B25" s="3" t="s">
         <v>294</v>
@@ -2542,22 +2537,22 @@
       <selection activeCell="I38" sqref="I38:J38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="22.33203125" customWidth="1"/>
     <col min="2" max="2" width="8" customWidth="1"/>
-    <col min="3" max="3" width="21.77734375" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" customWidth="1"/>
-    <col min="6" max="6" width="15.44140625" customWidth="1"/>
-    <col min="7" max="7" width="30.77734375" customWidth="1"/>
-    <col min="8" max="8" width="27.77734375" customWidth="1"/>
-    <col min="9" max="9" width="12.44140625" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" customWidth="1"/>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" customWidth="1"/>
+    <col min="6" max="6" width="15.5" customWidth="1"/>
+    <col min="7" max="7" width="30.83203125" customWidth="1"/>
+    <col min="8" max="8" width="27.83203125" customWidth="1"/>
+    <col min="9" max="9" width="12.5" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
-    <col min="11" max="11" width="16.77734375" customWidth="1"/>
+    <col min="11" max="11" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="45" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" s="45" customFormat="1" ht="30">
       <c r="A1" s="44" t="s">
         <v>77</v>
       </c>
@@ -2596,7 +2591,7 @@
       <c r="N1" s="44"/>
       <c r="O1" s="44"/>
     </row>
-    <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" s="1" customFormat="1">
       <c r="A2" s="3"/>
       <c r="D2" s="1" t="s">
         <v>5</v>
@@ -2610,7 +2605,7 @@
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
     </row>
-    <row r="3" spans="1:15" s="1" customFormat="1" ht="94.25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" s="1" customFormat="1" ht="90">
       <c r="A3" s="3"/>
       <c r="D3" s="1" t="s">
         <v>34</v>
@@ -2630,7 +2625,7 @@
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
     </row>
-    <row r="4" spans="1:15" s="10" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" s="10" customFormat="1" ht="30">
       <c r="A4" s="9"/>
       <c r="B4" s="10" t="s">
         <v>118</v>
@@ -2644,7 +2639,7 @@
       <c r="N4" s="9"/>
       <c r="O4" s="9"/>
     </row>
-    <row r="5" spans="1:15" s="10" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" s="10" customFormat="1" ht="30">
       <c r="A5" s="9"/>
       <c r="D5" s="10" t="s">
         <v>31</v>
@@ -2664,7 +2659,7 @@
       <c r="N5" s="9"/>
       <c r="O5" s="9"/>
     </row>
-    <row r="6" spans="1:15" s="10" customFormat="1" ht="78.55" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" s="10" customFormat="1" ht="75">
       <c r="A6" s="9"/>
       <c r="D6" s="10" t="s">
         <v>1</v>
@@ -2689,7 +2684,7 @@
       <c r="N6" s="9"/>
       <c r="O6" s="9"/>
     </row>
-    <row r="7" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" s="10" customFormat="1">
       <c r="A7" s="9"/>
       <c r="B7" s="10" t="s">
         <v>123</v>
@@ -2700,7 +2695,7 @@
       <c r="N7" s="9"/>
       <c r="O7" s="9"/>
     </row>
-    <row r="8" spans="1:15" s="10" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" s="10" customFormat="1" ht="30">
       <c r="A8" s="9"/>
       <c r="D8" s="10" t="s">
         <v>235</v>
@@ -2720,7 +2715,7 @@
       <c r="N8" s="9"/>
       <c r="O8" s="9"/>
     </row>
-    <row r="9" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" s="10" customFormat="1">
       <c r="A9" s="9"/>
       <c r="B9" s="10" t="s">
         <v>70</v>
@@ -2731,7 +2726,7 @@
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
     </row>
-    <row r="10" spans="1:15" s="1" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" s="1" customFormat="1" ht="45">
       <c r="A10" s="3"/>
       <c r="D10" s="1" t="s">
         <v>34</v>
@@ -2751,7 +2746,7 @@
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
     </row>
-    <row r="11" spans="1:15" s="12" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" s="12" customFormat="1" ht="30">
       <c r="A11" s="11"/>
       <c r="B11" s="12" t="s">
         <v>118</v>
@@ -2765,7 +2760,7 @@
       <c r="N11" s="11"/>
       <c r="O11" s="11"/>
     </row>
-    <row r="12" spans="1:15" s="12" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" s="12" customFormat="1" ht="30">
       <c r="A12" s="11"/>
       <c r="D12" s="12" t="s">
         <v>31</v>
@@ -2785,7 +2780,7 @@
       <c r="N12" s="11"/>
       <c r="O12" s="11"/>
     </row>
-    <row r="13" spans="1:15" s="12" customFormat="1" ht="78.55" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" s="12" customFormat="1" ht="75">
       <c r="A13" s="11"/>
       <c r="D13" s="12" t="s">
         <v>1</v>
@@ -2810,7 +2805,7 @@
       <c r="N13" s="11"/>
       <c r="O13" s="11"/>
     </row>
-    <row r="14" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" s="12" customFormat="1">
       <c r="A14" s="11"/>
       <c r="B14" s="12" t="s">
         <v>70</v>
@@ -2821,7 +2816,7 @@
       <c r="N14" s="11"/>
       <c r="O14" s="11"/>
     </row>
-    <row r="15" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" s="28" customFormat="1">
       <c r="A15" s="27"/>
       <c r="K15" s="27"/>
       <c r="L15" s="27"/>
@@ -2829,7 +2824,7 @@
       <c r="N15" s="27"/>
       <c r="O15" s="27"/>
     </row>
-    <row r="16" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" s="1" customFormat="1">
       <c r="A16" s="3"/>
       <c r="D16" s="1" t="s">
         <v>5</v>
@@ -2843,7 +2838,7 @@
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
     </row>
-    <row r="17" spans="1:15" s="1" customFormat="1" ht="62.85" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" s="1" customFormat="1" ht="60">
       <c r="A17" s="3"/>
       <c r="D17" s="1" t="s">
         <v>34</v>
@@ -2863,7 +2858,7 @@
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
     </row>
-    <row r="18" spans="1:15" s="26" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" s="26" customFormat="1" ht="30">
       <c r="A18" s="16"/>
       <c r="B18" s="26" t="s">
         <v>118</v>
@@ -2877,7 +2872,7 @@
       <c r="N18" s="16"/>
       <c r="O18" s="16"/>
     </row>
-    <row r="19" spans="1:15" s="26" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" s="26" customFormat="1" ht="30">
       <c r="A19" s="16"/>
       <c r="D19" s="26" t="s">
         <v>31</v>
@@ -2897,7 +2892,7 @@
       <c r="N19" s="16"/>
       <c r="O19" s="16"/>
     </row>
-    <row r="20" spans="1:15" s="26" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" s="26" customFormat="1" ht="30">
       <c r="A20" s="16"/>
       <c r="D20" s="26" t="s">
         <v>34</v>
@@ -2917,7 +2912,7 @@
       <c r="N20" s="16"/>
       <c r="O20" s="16"/>
     </row>
-    <row r="21" spans="1:15" s="10" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" s="10" customFormat="1" ht="30">
       <c r="A21" s="9"/>
       <c r="B21" s="10" t="s">
         <v>68</v>
@@ -2931,7 +2926,7 @@
       <c r="N21" s="9"/>
       <c r="O21" s="9"/>
     </row>
-    <row r="22" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" s="10" customFormat="1">
       <c r="A22" s="9"/>
       <c r="D22" s="10" t="s">
         <v>31</v>
@@ -2951,7 +2946,7 @@
       <c r="N22" s="9"/>
       <c r="O22" s="9"/>
     </row>
-    <row r="23" spans="1:15" s="8" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" s="8" customFormat="1" ht="30">
       <c r="A23" s="7"/>
       <c r="B23" s="8" t="s">
         <v>118</v>
@@ -2965,7 +2960,7 @@
       <c r="N23" s="7"/>
       <c r="O23" s="7"/>
     </row>
-    <row r="24" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" s="8" customFormat="1">
       <c r="A24" s="7"/>
       <c r="D24" s="8" t="s">
         <v>18</v>
@@ -2982,7 +2977,7 @@
       <c r="N24" s="7"/>
       <c r="O24" s="7"/>
     </row>
-    <row r="25" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" s="8" customFormat="1">
       <c r="A25" s="7"/>
       <c r="B25" s="8" t="s">
         <v>70</v>
@@ -2993,7 +2988,7 @@
       <c r="N25" s="7"/>
       <c r="O25" s="7"/>
     </row>
-    <row r="26" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" s="10" customFormat="1">
       <c r="A26" s="9"/>
       <c r="B26" s="10" t="s">
         <v>70</v>
@@ -3004,7 +2999,7 @@
       <c r="N26" s="9"/>
       <c r="O26" s="9"/>
     </row>
-    <row r="27" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" s="26" customFormat="1">
       <c r="A27" s="16"/>
       <c r="B27" s="26" t="s">
         <v>70</v>
@@ -3015,7 +3010,7 @@
       <c r="N27" s="16"/>
       <c r="O27" s="16"/>
     </row>
-    <row r="28" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" s="1" customFormat="1">
       <c r="A28" s="3"/>
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
@@ -3023,7 +3018,7 @@
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
     </row>
-    <row r="29" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" s="1" customFormat="1">
       <c r="A29" s="3"/>
       <c r="D29" s="1" t="s">
         <v>5</v>
@@ -3036,7 +3031,7 @@
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
     </row>
-    <row r="30" spans="1:15" s="1" customFormat="1" ht="62.85" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" s="1" customFormat="1" ht="60">
       <c r="A30" s="3"/>
       <c r="D30" s="1" t="s">
         <v>34</v>
@@ -3056,7 +3051,7 @@
       <c r="N30" s="3"/>
       <c r="O30" s="3"/>
     </row>
-    <row r="31" spans="1:15" s="12" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" s="12" customFormat="1" ht="30">
       <c r="A31" s="11"/>
       <c r="B31" s="12" t="s">
         <v>68</v>
@@ -3070,7 +3065,7 @@
       <c r="N31" s="11"/>
       <c r="O31" s="11"/>
     </row>
-    <row r="32" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" s="12" customFormat="1">
       <c r="A32" s="11"/>
       <c r="D32" s="12" t="s">
         <v>1</v>
@@ -3088,7 +3083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" s="12" customFormat="1">
       <c r="A33" s="11"/>
       <c r="B33" s="12" t="s">
         <v>70</v>
@@ -3099,7 +3094,7 @@
       <c r="N33" s="11"/>
       <c r="O33" s="11"/>
     </row>
-    <row r="34" spans="1:15" s="30" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" s="30" customFormat="1" ht="45">
       <c r="A34" s="29" t="s">
         <v>304</v>
       </c>
@@ -3122,7 +3117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" s="1" customFormat="1">
       <c r="A35" s="3"/>
       <c r="D35" s="1" t="s">
         <v>5</v>
@@ -3136,7 +3131,7 @@
       <c r="N35" s="3"/>
       <c r="O35" s="3"/>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15">
       <c r="D36" s="1" t="s">
         <v>1</v>
       </c>
@@ -3153,7 +3148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15">
       <c r="D37" s="1" t="s">
         <v>5</v>
       </c>
@@ -3161,7 +3156,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15">
       <c r="D38" s="1" t="s">
         <v>1</v>
       </c>
@@ -3197,18 +3192,18 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" customWidth="1"/>
-    <col min="3" max="3" width="33.77734375" customWidth="1"/>
+    <col min="1" max="1" width="22.5" customWidth="1"/>
+    <col min="3" max="3" width="33.83203125" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" customWidth="1"/>
-    <col min="6" max="6" width="21.44140625" customWidth="1"/>
+    <col min="6" max="6" width="21.5" customWidth="1"/>
     <col min="7" max="7" width="38.6640625" customWidth="1"/>
     <col min="8" max="8" width="54" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="45" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="45" customFormat="1">
       <c r="A1" s="44" t="s">
         <v>77</v>
       </c>
@@ -3239,7 +3234,7 @@
       <c r="L1" s="44"/>
       <c r="M1" s="44"/>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" ht="105.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" s="1" customFormat="1" ht="105">
       <c r="A2" s="3"/>
       <c r="D2" s="1" t="s">
         <v>5</v>
@@ -3256,7 +3251,7 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" s="1" customFormat="1" ht="30">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -3278,7 +3273,7 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:13" s="32" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" s="32" customFormat="1" ht="45">
       <c r="A4" s="31" t="s">
         <v>76</v>
       </c>
@@ -3296,7 +3291,7 @@
       <c r="L4" s="31"/>
       <c r="M4" s="31"/>
     </row>
-    <row r="5" spans="1:13" s="32" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" s="32" customFormat="1" ht="30">
       <c r="A5" s="31" t="s">
         <v>75</v>
       </c>
@@ -3318,7 +3313,7 @@
       <c r="L5" s="31"/>
       <c r="M5" s="31"/>
     </row>
-    <row r="6" spans="1:13" s="10" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" s="10" customFormat="1" ht="30">
       <c r="A6" s="9"/>
       <c r="B6" s="9" t="s">
         <v>68</v>
@@ -3336,7 +3331,7 @@
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
     </row>
-    <row r="7" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" s="10" customFormat="1">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -3358,7 +3353,7 @@
       <c r="L7" s="9"/>
       <c r="M7" s="9"/>
     </row>
-    <row r="8" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" s="10" customFormat="1">
       <c r="A8" s="9"/>
       <c r="B8" s="9" t="s">
         <v>70</v>
@@ -3374,7 +3369,7 @@
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
     </row>
-    <row r="9" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" s="32" customFormat="1">
       <c r="A9" s="31"/>
       <c r="B9" s="31" t="s">
         <v>47</v>
@@ -3390,7 +3385,7 @@
       <c r="L9" s="31"/>
       <c r="M9" s="31"/>
     </row>
-    <row r="10" spans="1:13" s="1" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" s="1" customFormat="1" ht="30">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -3412,7 +3407,7 @@
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
     </row>
-    <row r="11" spans="1:13" s="25" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" s="25" customFormat="1" ht="30">
       <c r="A11" s="17"/>
       <c r="B11" s="17" t="s">
         <v>46</v>
@@ -3428,7 +3423,7 @@
       <c r="L11" s="17"/>
       <c r="M11" s="17"/>
     </row>
-    <row r="12" spans="1:13" s="25" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" s="25" customFormat="1" ht="30">
       <c r="A12" s="17"/>
       <c r="B12" s="17"/>
       <c r="C12" s="17"/>
@@ -3450,7 +3445,7 @@
       <c r="L12" s="17"/>
       <c r="M12" s="17"/>
     </row>
-    <row r="13" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" s="10" customFormat="1">
       <c r="A13" s="9"/>
       <c r="B13" s="9" t="s">
         <v>68</v>
@@ -3468,7 +3463,7 @@
       <c r="L13" s="9"/>
       <c r="M13" s="9"/>
     </row>
-    <row r="14" spans="1:13" s="10" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" s="10" customFormat="1" ht="30">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
@@ -3490,7 +3485,7 @@
       <c r="L14" s="9"/>
       <c r="M14" s="9"/>
     </row>
-    <row r="15" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" s="10" customFormat="1">
       <c r="A15" s="9"/>
       <c r="B15" s="9" t="s">
         <v>70</v>
@@ -3506,7 +3501,7 @@
       <c r="L15" s="9"/>
       <c r="M15" s="9"/>
     </row>
-    <row r="16" spans="1:13" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" s="25" customFormat="1">
       <c r="A16" s="17"/>
       <c r="B16" s="17" t="s">
         <v>47</v>
@@ -3522,7 +3517,7 @@
       <c r="L16" s="17"/>
       <c r="M16" s="17"/>
     </row>
-    <row r="17" spans="1:13" s="1" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" s="1" customFormat="1" ht="30">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -3544,7 +3539,7 @@
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
     </row>
-    <row r="18" spans="1:13" s="12" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" s="12" customFormat="1" ht="30">
       <c r="A18" s="11"/>
       <c r="B18" s="11" t="s">
         <v>68</v>
@@ -3562,7 +3557,7 @@
       <c r="L18" s="11"/>
       <c r="M18" s="11"/>
     </row>
-    <row r="19" spans="1:13" s="12" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" s="12" customFormat="1" ht="30">
       <c r="A19" s="11" t="s">
         <v>74</v>
       </c>
@@ -3584,7 +3579,7 @@
       <c r="L19" s="11"/>
       <c r="M19" s="11"/>
     </row>
-    <row r="20" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" s="12" customFormat="1">
       <c r="A20" s="11"/>
       <c r="B20" s="11" t="s">
         <v>70</v>
@@ -3600,7 +3595,7 @@
       <c r="L20" s="11"/>
       <c r="M20" s="11"/>
     </row>
-    <row r="21" spans="1:13" s="1" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" s="1" customFormat="1" ht="30">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -3622,7 +3617,7 @@
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
     </row>
-    <row r="22" spans="1:13" s="1" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" s="1" customFormat="1" ht="30">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -3663,19 +3658,19 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="23.77734375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.83203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="19.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="29.33203125" style="1" customWidth="1"/>
-    <col min="4" max="6" width="14.44140625" style="1" customWidth="1"/>
+    <col min="4" max="6" width="14.5" style="1" customWidth="1"/>
     <col min="7" max="7" width="34" style="1" customWidth="1"/>
     <col min="8" max="8" width="32.33203125" style="1" customWidth="1"/>
-    <col min="9" max="13" width="10.77734375" style="3"/>
-    <col min="14" max="16384" width="10.77734375" style="1"/>
+    <col min="9" max="13" width="10.83203125" style="3"/>
+    <col min="14" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="45" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="45" customFormat="1">
       <c r="A1" s="44" t="s">
         <v>77</v>
       </c>
@@ -3706,7 +3701,7 @@
       <c r="L1" s="44"/>
       <c r="M1" s="44"/>
     </row>
-    <row r="2" spans="1:13" ht="47.15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="45">
       <c r="A2" s="3" t="s">
         <v>298</v>
       </c>
@@ -3720,7 +3715,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="6" customFormat="1" ht="62.85" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" s="6" customFormat="1" ht="60">
       <c r="A5" s="5" t="s">
         <v>312</v>
       </c>
@@ -3733,7 +3728,7 @@
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
     </row>
-    <row r="7" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" s="6" customFormat="1">
       <c r="A7" s="5"/>
       <c r="B7" s="6" t="s">
         <v>103</v>
@@ -3744,7 +3739,7 @@
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
     </row>
-    <row r="9" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" s="6" customFormat="1">
       <c r="A9" s="5"/>
       <c r="B9" s="6" t="s">
         <v>130</v>
@@ -3755,7 +3750,7 @@
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
     </row>
-    <row r="11" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" s="6" customFormat="1">
       <c r="A11" s="5"/>
       <c r="B11" s="6" t="s">
         <v>136</v>
@@ -3766,7 +3761,7 @@
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
     </row>
-    <row r="13" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" s="6" customFormat="1">
       <c r="A13" s="5"/>
       <c r="B13" s="6" t="s">
         <v>138</v>
@@ -3777,7 +3772,7 @@
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
     </row>
-    <row r="15" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" s="6" customFormat="1">
       <c r="A15" s="5"/>
       <c r="B15" s="6" t="s">
         <v>104</v>
@@ -3788,7 +3783,7 @@
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
     </row>
-    <row r="17" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" s="6" customFormat="1">
       <c r="A17" s="5"/>
       <c r="B17" s="6" t="s">
         <v>137</v>
@@ -3818,14 +3813,14 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" customWidth="1"/>
+    <col min="1" max="1" width="19.5" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" customWidth="1"/>
-    <col min="3" max="3" width="26.44140625" customWidth="1"/>
+    <col min="3" max="3" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="46" customFormat="1">
       <c r="A1" s="46" t="s">
         <v>64</v>
       </c>
@@ -3836,7 +3831,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="37" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" s="37" customFormat="1">
       <c r="A2" s="37" t="s">
         <v>63</v>
       </c>
@@ -3847,7 +3842,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="37" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" s="37" customFormat="1">
       <c r="A3" s="37" t="s">
         <v>63</v>
       </c>
@@ -3858,7 +3853,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="38" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" s="38" customFormat="1">
       <c r="A4" s="16" t="s">
         <v>84</v>
       </c>
@@ -3869,7 +3864,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="38" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" s="38" customFormat="1">
       <c r="A5" s="16" t="s">
         <v>84</v>
       </c>
@@ -3880,7 +3875,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="39" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" s="39" customFormat="1">
       <c r="A6" s="7" t="s">
         <v>78</v>
       </c>
@@ -3891,7 +3886,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="39" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" s="39" customFormat="1">
       <c r="A7" s="7" t="s">
         <v>78</v>
       </c>
@@ -3902,7 +3897,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="39" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" s="39" customFormat="1">
       <c r="A8" s="7" t="s">
         <v>78</v>
       </c>
@@ -3913,7 +3908,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="40" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" s="40" customFormat="1">
       <c r="A9" s="9" t="s">
         <v>219</v>
       </c>
@@ -3924,7 +3919,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="40" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" s="40" customFormat="1">
       <c r="A10" s="9" t="s">
         <v>219</v>
       </c>
@@ -3935,7 +3930,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="40" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" s="40" customFormat="1">
       <c r="A11" s="9" t="s">
         <v>219</v>
       </c>
@@ -3946,7 +3941,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="40" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" s="40" customFormat="1">
       <c r="A12" s="9" t="s">
         <v>219</v>
       </c>
@@ -3957,7 +3952,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="40" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" s="40" customFormat="1">
       <c r="A13" s="9" t="s">
         <v>219</v>
       </c>
@@ -3968,7 +3963,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="40" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" s="40" customFormat="1">
       <c r="A14" s="9" t="s">
         <v>219</v>
       </c>
@@ -3979,7 +3974,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="40" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" s="40" customFormat="1" ht="30">
       <c r="A15" s="9" t="s">
         <v>219</v>
       </c>
@@ -3990,7 +3985,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="41" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" s="41" customFormat="1">
       <c r="A16" s="11" t="s">
         <v>251</v>
       </c>
@@ -4001,7 +3996,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="41" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" s="41" customFormat="1">
       <c r="A17" s="11" t="s">
         <v>251</v>
       </c>
@@ -4012,7 +4007,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="42" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" s="42" customFormat="1">
       <c r="A18" s="13" t="s">
         <v>253</v>
       </c>
@@ -4023,7 +4018,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="42" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" s="42" customFormat="1">
       <c r="A19" s="13" t="s">
         <v>253</v>
       </c>
@@ -4034,7 +4029,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="42" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" s="42" customFormat="1">
       <c r="A20" s="13" t="s">
         <v>253</v>
       </c>
@@ -4045,7 +4040,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" s="43" customFormat="1">
       <c r="A21" s="17" t="s">
         <v>268</v>
       </c>
@@ -4056,7 +4051,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" s="43" customFormat="1">
       <c r="A22" s="17" t="s">
         <v>268</v>
       </c>
@@ -4067,7 +4062,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" s="43" customFormat="1">
       <c r="A23" s="17" t="s">
         <v>268</v>
       </c>
@@ -4078,7 +4073,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="43" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" s="43" customFormat="1" ht="30">
       <c r="A24" s="17" t="s">
         <v>268</v>
       </c>
@@ -4104,20 +4099,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="19" style="3" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" style="3" customWidth="1"/>
     <col min="3" max="3" width="21.33203125" style="3" customWidth="1"/>
     <col min="4" max="4" width="36" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="10.77734375" style="3"/>
+    <col min="5" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="44" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="44" customFormat="1">
       <c r="A1" s="44" t="s">
         <v>11</v>
       </c>
@@ -4131,7 +4126,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
@@ -4140,7 +4135,7 @@
       </c>
       <c r="D2" s="48"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
@@ -4149,7 +4144,7 @@
       </c>
       <c r="D3" s="48"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
@@ -4158,7 +4153,7 @@
       </c>
       <c r="D4" s="48"/>
     </row>
-    <row r="5" spans="1:4" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
@@ -4167,7 +4162,7 @@
       </c>
       <c r="D5" s="48"/>
     </row>
-    <row r="6" spans="1:4" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="30">
       <c r="A6" s="3" t="s">
         <v>107</v>
       </c>
@@ -4178,7 +4173,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7" s="3" t="s">
         <v>109</v>
       </c>
@@ -4187,7 +4182,7 @@
       </c>
       <c r="D7" s="48"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="A8" s="3" t="s">
         <v>133</v>
       </c>
@@ -4196,7 +4191,7 @@
       </c>
       <c r="D8" s="48"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" s="3" t="s">
         <v>134</v>
       </c>
@@ -4205,7 +4200,7 @@
       </c>
       <c r="D9" s="48"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10" s="3" t="s">
         <v>141</v>
       </c>
@@ -4214,7 +4209,7 @@
       </c>
       <c r="D10" s="48"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4">
       <c r="A11" s="3" t="s">
         <v>177</v>
       </c>
@@ -4223,7 +4218,7 @@
       </c>
       <c r="D11" s="48"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4">
       <c r="A12" s="3" t="s">
         <v>179</v>
       </c>
@@ -4232,7 +4227,7 @@
       </c>
       <c r="D12" s="48"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="A13" s="3" t="s">
         <v>42</v>
       </c>
@@ -4260,20 +4255,20 @@
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="39.109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="39.1640625" style="3" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="15.77734375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" style="3" customWidth="1"/>
     <col min="4" max="4" width="21" style="3" customWidth="1"/>
     <col min="5" max="5" width="32.6640625" style="3" customWidth="1"/>
     <col min="6" max="6" width="24.33203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="23.44140625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="24.44140625" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="10.77734375" style="3"/>
+    <col min="7" max="7" width="23.5" style="3" customWidth="1"/>
+    <col min="8" max="8" width="24.5" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="45" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="45" customFormat="1">
       <c r="A1" s="44" t="s">
         <v>77</v>
       </c>
@@ -4304,7 +4299,7 @@
       <c r="L1" s="44"/>
       <c r="M1" s="44"/>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" ht="33.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" s="1" customFormat="1" ht="33" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -4320,7 +4315,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" ht="75.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" s="1" customFormat="1" ht="76" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>315</v>
       </c>
@@ -4345,7 +4340,7 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:13" s="1" customFormat="1" ht="109" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" s="1" customFormat="1" ht="109" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>299</v>
       </c>
@@ -4389,18 +4384,18 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" style="3"/>
-    <col min="2" max="2" width="12.44140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.77734375" style="3"/>
-    <col min="4" max="4" width="24.44140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="23.44140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="3"/>
+    <col min="2" max="2" width="12.5" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="3"/>
+    <col min="4" max="4" width="24.5" style="3" customWidth="1"/>
+    <col min="5" max="5" width="23.5" style="3" customWidth="1"/>
     <col min="6" max="6" width="29.6640625" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="10.77734375" style="3"/>
+    <col min="7" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="44" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="44" customFormat="1">
       <c r="A1" s="44" t="s">
         <v>77</v>
       </c>
@@ -4420,7 +4415,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -4435,7 +4430,7 @@
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:14" s="1" customFormat="1" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A3" s="3"/>
       <c r="B3" s="1" t="s">
         <v>1</v>
@@ -4457,7 +4452,7 @@
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" s="1" customFormat="1">
       <c r="A4" s="3"/>
       <c r="C4" s="3"/>
       <c r="G4" s="3"/>
@@ -4484,18 +4479,18 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="24.109375" customWidth="1"/>
-    <col min="2" max="2" width="15.77734375" customWidth="1"/>
+    <col min="1" max="1" width="24.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="18.33203125" customWidth="1"/>
-    <col min="5" max="5" width="31.109375" customWidth="1"/>
-    <col min="6" max="6" width="23.109375" customWidth="1"/>
-    <col min="7" max="7" width="25.77734375" customWidth="1"/>
+    <col min="5" max="5" width="31.1640625" customWidth="1"/>
+    <col min="6" max="6" width="23.1640625" customWidth="1"/>
+    <col min="7" max="7" width="25.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="46" customFormat="1">
       <c r="A1" s="44" t="s">
         <v>77</v>
       </c>
@@ -4522,7 +4517,7 @@
       <c r="J1" s="44"/>
       <c r="K1" s="44"/>
     </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" s="1" customFormat="1">
       <c r="A2" s="3"/>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -4536,7 +4531,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:12" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="30">
       <c r="A3" s="3"/>
       <c r="B3" s="1" t="s">
         <v>1</v>
@@ -4559,7 +4554,7 @@
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:12" s="3" customFormat="1" ht="94.25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" s="3" customFormat="1" ht="90">
       <c r="A4" s="3" t="s">
         <v>300</v>
       </c>
@@ -4579,7 +4574,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="3" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" s="3" customFormat="1" ht="45">
       <c r="B5" s="3" t="s">
         <v>31</v>
       </c>
@@ -4593,7 +4588,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="3" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" s="3" customFormat="1" ht="45">
       <c r="B6" s="3" t="s">
         <v>31</v>
       </c>
@@ -4607,7 +4602,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="3" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" s="3" customFormat="1" ht="30">
       <c r="B7" s="3" t="s">
         <v>31</v>
       </c>
@@ -4621,7 +4616,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="3" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" s="3" customFormat="1" ht="30">
       <c r="B8" s="3" t="s">
         <v>31</v>
       </c>
@@ -4635,7 +4630,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="3" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" s="3" customFormat="1" ht="45">
       <c r="B9" s="3" t="s">
         <v>31</v>
       </c>
@@ -4649,7 +4644,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="3" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" s="3" customFormat="1" ht="45">
       <c r="B10" s="3" t="s">
         <v>31</v>
       </c>
@@ -4663,7 +4658,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="3" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" s="3" customFormat="1" ht="30">
       <c r="B11" s="3" t="s">
         <v>31</v>
       </c>
@@ -4680,7 +4675,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -4693,7 +4688,7 @@
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -4706,7 +4701,7 @@
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -4719,7 +4714,7 @@
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -4732,7 +4727,7 @@
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -4745,7 +4740,7 @@
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -4758,7 +4753,7 @@
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -4771,7 +4766,7 @@
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -4784,7 +4779,7 @@
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -4797,7 +4792,7 @@
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -4810,7 +4805,7 @@
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -4823,7 +4818,7 @@
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -4836,7 +4831,7 @@
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -4849,7 +4844,7 @@
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -4881,22 +4876,22 @@
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="37.6640625" style="3" customWidth="1"/>
     <col min="2" max="2" width="8.33203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="33.77734375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="13.77734375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="10.77734375" style="3"/>
+    <col min="3" max="3" width="33.83203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="3"/>
     <col min="6" max="6" width="14.6640625" style="3" customWidth="1"/>
     <col min="7" max="7" width="28.6640625" style="3" customWidth="1"/>
     <col min="8" max="8" width="12.33203125" customWidth="1"/>
     <col min="9" max="9" width="13.33203125" customWidth="1"/>
-    <col min="10" max="10" width="28.44140625" style="3" customWidth="1"/>
-    <col min="11" max="16384" width="10.77734375" style="3"/>
+    <col min="10" max="10" width="28.5" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="45" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="45" customFormat="1" ht="30">
       <c r="A1" s="44" t="s">
         <v>77</v>
       </c>
@@ -4931,7 +4926,7 @@
       <c r="L1" s="44"/>
       <c r="M1" s="44"/>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" s="1" customFormat="1" ht="30">
       <c r="A2" s="3"/>
       <c r="D2" s="1" t="s">
         <v>5</v>
@@ -4945,7 +4940,7 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" s="1" customFormat="1" ht="30">
       <c r="A3" s="3"/>
       <c r="D3" s="3" t="s">
         <v>34</v>
@@ -4964,7 +4959,7 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" s="8" customFormat="1">
       <c r="A4" s="7"/>
       <c r="B4" s="7" t="s">
         <v>118</v>
@@ -4981,7 +4976,7 @@
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
     </row>
-    <row r="5" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" s="8" customFormat="1">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -5004,7 +4999,7 @@
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
     </row>
-    <row r="6" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" s="8" customFormat="1">
       <c r="A6" s="7"/>
       <c r="B6" s="8" t="s">
         <v>123</v>
@@ -5020,7 +5015,7 @@
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
     </row>
-    <row r="7" spans="1:13" s="8" customFormat="1" ht="62.85" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" s="8" customFormat="1" ht="60">
       <c r="A7" s="7"/>
       <c r="D7" s="7" t="s">
         <v>34</v>
@@ -5041,7 +5036,7 @@
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
     </row>
-    <row r="8" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" s="10" customFormat="1">
       <c r="A8" s="9"/>
       <c r="B8" s="10" t="s">
         <v>68</v>
@@ -5060,7 +5055,7 @@
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
     </row>
-    <row r="9" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" s="10" customFormat="1">
       <c r="A9" s="9"/>
       <c r="D9" s="9" t="s">
         <v>31</v>
@@ -5081,7 +5076,7 @@
       <c r="L9" s="9"/>
       <c r="M9" s="9"/>
     </row>
-    <row r="10" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" s="10" customFormat="1">
       <c r="A10" s="9"/>
       <c r="B10" s="10" t="s">
         <v>70</v>
@@ -5097,7 +5092,7 @@
       <c r="L10" s="9"/>
       <c r="M10" s="9"/>
     </row>
-    <row r="11" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" s="8" customFormat="1">
       <c r="A11" s="7"/>
       <c r="B11" s="8" t="s">
         <v>70</v>
@@ -5113,7 +5108,7 @@
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
     </row>
-    <row r="12" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" s="14" customFormat="1">
       <c r="A12" s="13"/>
       <c r="B12" s="14" t="s">
         <v>118</v>
@@ -5128,7 +5123,7 @@
       <c r="L12" s="13"/>
       <c r="M12" s="13"/>
     </row>
-    <row r="13" spans="1:13" s="14" customFormat="1" ht="94.25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" s="14" customFormat="1" ht="90">
       <c r="A13" s="13" t="s">
         <v>301</v>
       </c>
@@ -5154,7 +5149,7 @@
       <c r="L13" s="13"/>
       <c r="M13" s="13"/>
     </row>
-    <row r="14" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" s="14" customFormat="1">
       <c r="A14" s="13"/>
       <c r="B14" s="14" t="s">
         <v>70</v>
@@ -5166,43 +5161,43 @@
       <c r="L14" s="13"/>
       <c r="M14" s="13"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13">
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13">
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="8:9">
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="8:9">
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="8:9">
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="8:9">
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
     </row>
-    <row r="21" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="8:9">
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="8:9">
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="8:9">
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
     </row>
-    <row r="24" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="8:9">
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
     </row>
@@ -5225,22 +5220,22 @@
       <selection activeCell="I25" sqref="I25:J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="29.77734375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="10.77734375" style="3"/>
-    <col min="3" max="3" width="29.109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="15.109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="10.77734375" style="3"/>
+    <col min="1" max="1" width="29.83203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="3"/>
+    <col min="3" max="3" width="29.1640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="3"/>
     <col min="6" max="6" width="25.33203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="35.77734375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="25.44140625" style="3" customWidth="1"/>
-    <col min="9" max="10" width="10.77734375" style="3"/>
+    <col min="7" max="7" width="35.83203125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="25.5" style="3" customWidth="1"/>
+    <col min="9" max="10" width="10.83203125" style="3"/>
     <col min="11" max="11" width="21.6640625" style="3" customWidth="1"/>
-    <col min="12" max="16384" width="10.77734375" style="3"/>
+    <col min="12" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="45" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="45" customFormat="1" ht="45">
       <c r="A1" s="44" t="s">
         <v>77</v>
       </c>
@@ -5278,7 +5273,7 @@
       <c r="M1" s="44"/>
       <c r="N1" s="44"/>
     </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" ht="94.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" s="1" customFormat="1" ht="90">
       <c r="A2" s="18"/>
       <c r="B2" s="19"/>
       <c r="C2" s="19"/>
@@ -5299,7 +5294,7 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:14" ht="47.15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="45">
       <c r="A3" s="18"/>
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
@@ -5320,7 +5315,7 @@
       <c r="J3" s="18"/>
       <c r="K3" s="18"/>
     </row>
-    <row r="4" spans="1:14" s="16" customFormat="1" ht="94.25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" s="16" customFormat="1" ht="90">
       <c r="A4" s="20" t="s">
         <v>302</v>
       </c>
@@ -5339,7 +5334,7 @@
       <c r="J4" s="20"/>
       <c r="K4" s="20"/>
     </row>
-    <row r="5" spans="1:14" s="16" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" s="16" customFormat="1" ht="45">
       <c r="A5" s="20"/>
       <c r="B5" s="20"/>
       <c r="C5" s="20"/>
@@ -5364,7 +5359,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="16" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" s="16" customFormat="1" ht="30">
       <c r="A6" s="20"/>
       <c r="B6" s="20"/>
       <c r="C6" s="20"/>
@@ -5385,7 +5380,7 @@
       <c r="J6" s="20"/>
       <c r="K6" s="20"/>
     </row>
-    <row r="7" spans="1:14" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" s="17" customFormat="1">
       <c r="A7" s="21"/>
       <c r="B7" s="21" t="s">
         <v>68</v>
@@ -5402,7 +5397,7 @@
       <c r="J7" s="21"/>
       <c r="K7" s="21"/>
     </row>
-    <row r="8" spans="1:14" s="17" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" s="17" customFormat="1" ht="30">
       <c r="A8" s="21"/>
       <c r="B8" s="21"/>
       <c r="C8" s="21"/>
@@ -5423,7 +5418,7 @@
       <c r="J8" s="21"/>
       <c r="K8" s="21"/>
     </row>
-    <row r="9" spans="1:14" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" s="17" customFormat="1">
       <c r="A9" s="21"/>
       <c r="B9" s="21" t="s">
         <v>70</v>
@@ -5438,7 +5433,7 @@
       <c r="J9" s="21"/>
       <c r="K9" s="21"/>
     </row>
-    <row r="10" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" s="16" customFormat="1">
       <c r="A10" s="20"/>
       <c r="B10" s="20" t="s">
         <v>70</v>
@@ -5453,7 +5448,7 @@
       <c r="J10" s="20"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="1:14" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="30">
       <c r="A11" s="18"/>
       <c r="B11" s="18"/>
       <c r="C11" s="18"/>
@@ -5474,7 +5469,7 @@
       <c r="J11" s="18"/>
       <c r="K11" s="18"/>
     </row>
-    <row r="12" spans="1:14" s="9" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" s="9" customFormat="1" ht="45">
       <c r="A12" s="22"/>
       <c r="B12" s="22" t="s">
         <v>68</v>
@@ -5491,7 +5486,7 @@
       <c r="J12" s="22"/>
       <c r="K12" s="22"/>
     </row>
-    <row r="13" spans="1:14" s="9" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" s="9" customFormat="1" ht="45">
       <c r="A13" s="22"/>
       <c r="B13" s="22"/>
       <c r="C13" s="22"/>
@@ -5516,7 +5511,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="14" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" s="9" customFormat="1">
       <c r="A14" s="22"/>
       <c r="B14" s="22" t="s">
         <v>70</v>
@@ -5531,7 +5526,7 @@
       <c r="J14" s="22"/>
       <c r="K14" s="22"/>
     </row>
-    <row r="15" spans="1:14" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="30">
       <c r="A15" s="18"/>
       <c r="B15" s="18"/>
       <c r="C15" s="18"/>
@@ -5552,7 +5547,7 @@
       <c r="J15" s="18"/>
       <c r="K15" s="18"/>
     </row>
-    <row r="16" spans="1:14" s="11" customFormat="1" ht="62.85" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" s="11" customFormat="1" ht="60">
       <c r="A16" s="23"/>
       <c r="B16" s="23" t="s">
         <v>118</v>
@@ -5569,7 +5564,7 @@
       <c r="J16" s="23"/>
       <c r="K16" s="23"/>
     </row>
-    <row r="17" spans="1:11" s="11" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" s="11" customFormat="1" ht="45">
       <c r="A17" s="23"/>
       <c r="B17" s="23"/>
       <c r="C17" s="23"/>
@@ -5594,7 +5589,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="18" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" s="11" customFormat="1">
       <c r="A18" s="23"/>
       <c r="B18" s="23" t="s">
         <v>70</v>
@@ -5609,7 +5604,7 @@
       <c r="J18" s="23"/>
       <c r="K18" s="23"/>
     </row>
-    <row r="19" spans="1:11" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" ht="30">
       <c r="A19" s="18"/>
       <c r="B19" s="18"/>
       <c r="C19" s="18"/>
@@ -5630,7 +5625,7 @@
       <c r="J19" s="18"/>
       <c r="K19" s="18"/>
     </row>
-    <row r="20" spans="1:11" s="5" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" s="5" customFormat="1" ht="45">
       <c r="A20" s="24"/>
       <c r="B20" s="24" t="s">
         <v>118</v>
@@ -5647,7 +5642,7 @@
       <c r="J20" s="24"/>
       <c r="K20" s="24"/>
     </row>
-    <row r="21" spans="1:11" s="5" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" s="5" customFormat="1" ht="45">
       <c r="A21" s="24"/>
       <c r="B21" s="24"/>
       <c r="C21" s="24"/>
@@ -5672,7 +5667,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="22" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" s="5" customFormat="1">
       <c r="A22" s="24"/>
       <c r="B22" s="24" t="s">
         <v>70</v>
@@ -5687,7 +5682,7 @@
       <c r="J22" s="24"/>
       <c r="K22" s="24"/>
     </row>
-    <row r="23" spans="1:11" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" ht="30">
       <c r="A23" s="18"/>
       <c r="B23" s="18"/>
       <c r="C23" s="18"/>
@@ -5708,7 +5703,7 @@
       <c r="J23" s="18"/>
       <c r="K23" s="18"/>
     </row>
-    <row r="24" spans="1:11" s="17" customFormat="1" ht="62.85" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" s="17" customFormat="1" ht="60">
       <c r="A24" s="21"/>
       <c r="B24" s="21" t="s">
         <v>118</v>
@@ -5725,7 +5720,7 @@
       <c r="J24" s="21"/>
       <c r="K24" s="21"/>
     </row>
-    <row r="25" spans="1:11" s="17" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" s="17" customFormat="1" ht="45">
       <c r="A25" s="21"/>
       <c r="B25" s="21"/>
       <c r="C25" s="21"/>
@@ -5750,7 +5745,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="26" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" s="17" customFormat="1">
       <c r="A26" s="21"/>
       <c r="B26" s="21" t="s">
         <v>70</v>
@@ -5765,7 +5760,7 @@
       <c r="J26" s="21"/>
       <c r="K26" s="21"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11">
       <c r="A27" s="18"/>
       <c r="B27" s="18"/>
       <c r="C27" s="18"/>
@@ -5782,7 +5777,7 @@
       <c r="J27" s="18"/>
       <c r="K27" s="18"/>
     </row>
-    <row r="28" spans="1:11" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" s="29" customFormat="1">
       <c r="A28" s="47" t="s">
         <v>206</v>
       </c>

</xml_diff>

<commit_message>
Initial check-in of translations changes.
</commit_message>
<xml_diff>
--- a/app/config/tables/Ethiopia_household/forms/Ethiopia_household/Ethiopia_household.xlsx
+++ b/app/config/tables/Ethiopia_household/forms/Ethiopia_household/Ethiopia_household.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\toolsuite\app-designer\app\config\tables\Ethiopia_household\forms\Ethiopia_household\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="60" yWindow="0" windowWidth="30740" windowHeight="16660" tabRatio="500"/>
+    <workbookView xWindow="65" yWindow="0" windowWidth="30737" windowHeight="16665" tabRatio="500" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="queries" sheetId="9" r:id="rId1"/>
@@ -29,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="319">
   <si>
     <t>type</t>
   </si>
@@ -52,9 +57,6 @@
     <t>Section 2: HOUSEHOLD DEMOGRAPHICS</t>
   </si>
   <si>
-    <t>display.hint</t>
-  </si>
-  <si>
     <t>Ask of household head or knowledgeable household member</t>
   </si>
   <si>
@@ -70,9 +72,6 @@
     <t>value</t>
   </si>
   <si>
-    <t>display.title</t>
-  </si>
-  <si>
     <t>form_id</t>
   </si>
   <si>
@@ -199,9 +198,6 @@
     <t>Add House Member</t>
   </si>
   <si>
-    <t>display.new_instance_text</t>
-  </si>
-  <si>
     <t>Section 9.3 Health</t>
   </si>
   <si>
@@ -983,12 +979,24 @@
   </si>
   <si>
     <t>'household_id='+opendatakit.encodeURIDataElement('household_id')</t>
+  </si>
+  <si>
+    <t>display.hint.text</t>
+  </si>
+  <si>
+    <t>display.prompt.text</t>
+  </si>
+  <si>
+    <t>display.title.text</t>
+  </si>
+  <si>
+    <t>display.new_instance_label.text</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1941,51 +1949,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C8" workbookViewId="0">
+    <sheetView topLeftCell="C8" workbookViewId="0">
       <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.83203125" customWidth="1"/>
-    <col min="2" max="2" width="18.5" customWidth="1"/>
+    <col min="1" max="1" width="19.77734375" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" customWidth="1"/>
-    <col min="4" max="4" width="26.83203125" customWidth="1"/>
-    <col min="5" max="5" width="20.5" customWidth="1"/>
+    <col min="4" max="4" width="26.77734375" customWidth="1"/>
+    <col min="5" max="5" width="20.44140625" customWidth="1"/>
     <col min="6" max="6" width="23.33203125" customWidth="1"/>
-    <col min="7" max="7" width="26.1640625" customWidth="1"/>
+    <col min="7" max="7" width="26.109375" customWidth="1"/>
     <col min="8" max="8" width="39.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="46" customFormat="1">
+    <row r="1" spans="1:17" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="44" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B1" s="44" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C1" s="44" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D1" s="45" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F1" s="45" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="H1" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="45" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1">
+    </row>
+    <row r="2" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="36" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B2" s="33"/>
       <c r="C2" s="33"/>
@@ -1995,9 +2003,9 @@
       <c r="G2" s="34"/>
       <c r="H2" s="34"/>
     </row>
-    <row r="3" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1">
+    <row r="3" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="36" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B3" s="33"/>
       <c r="C3" s="33"/>
@@ -2007,9 +2015,9 @@
       <c r="G3" s="34"/>
       <c r="H3" s="34"/>
     </row>
-    <row r="4" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1">
+    <row r="4" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="36" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B4" s="33"/>
       <c r="C4" s="33"/>
@@ -2019,9 +2027,9 @@
       <c r="G4" s="34"/>
       <c r="H4" s="34"/>
     </row>
-    <row r="5" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1">
+    <row r="5" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="36" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B5" s="33"/>
       <c r="C5" s="33"/>
@@ -2031,9 +2039,9 @@
       <c r="G5" s="34"/>
       <c r="H5" s="34"/>
     </row>
-    <row r="6" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1">
+    <row r="6" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="36" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="33"/>
@@ -2043,9 +2051,9 @@
       <c r="G6" s="34"/>
       <c r="H6" s="34"/>
     </row>
-    <row r="7" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1">
+    <row r="7" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="36" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B7" s="33"/>
       <c r="C7" s="33"/>
@@ -2055,7 +2063,7 @@
       <c r="G7" s="34"/>
       <c r="H7" s="34"/>
     </row>
-    <row r="8" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1">
+    <row r="8" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="36"/>
       <c r="B8" s="33"/>
       <c r="C8" s="33"/>
@@ -2065,104 +2073,104 @@
       <c r="G8" s="34"/>
       <c r="H8" s="34"/>
     </row>
-    <row r="9" spans="1:17" ht="45">
+    <row r="9" spans="1:17" ht="47.15" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="H9" s="2" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="30">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" ht="30">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="H11" s="2" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" s="12" customFormat="1" ht="30" customHeight="1">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" s="12" customFormat="1" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>1</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="M12" s="11"/>
       <c r="N12" s="11"/>
@@ -2170,27 +2178,27 @@
       <c r="P12" s="11"/>
       <c r="Q12" s="11"/>
     </row>
-    <row r="13" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1">
+    <row r="13" spans="1:17" s="1" customFormat="1" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="H13" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
@@ -2198,27 +2206,27 @@
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
     </row>
-    <row r="14" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1">
+    <row r="14" spans="1:17" s="1" customFormat="1" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
@@ -2226,27 +2234,27 @@
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
     </row>
-    <row r="15" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1">
+    <row r="15" spans="1:17" s="1" customFormat="1" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
@@ -2254,27 +2262,27 @@
       <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
     </row>
-    <row r="16" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1">
+    <row r="16" spans="1:17" s="1" customFormat="1" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
@@ -2282,27 +2290,27 @@
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
     </row>
-    <row r="17" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1">
+    <row r="17" spans="1:17" s="1" customFormat="1" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
@@ -2310,27 +2318,27 @@
       <c r="P17" s="3"/>
       <c r="Q17" s="3"/>
     </row>
-    <row r="18" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1">
+    <row r="18" spans="1:17" s="1" customFormat="1" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
@@ -2338,27 +2346,27 @@
       <c r="P18" s="3"/>
       <c r="Q18" s="3"/>
     </row>
-    <row r="19" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1">
+    <row r="19" spans="1:17" s="1" customFormat="1" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>170</v>
-      </c>
       <c r="E19" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
@@ -2366,27 +2374,27 @@
       <c r="P19" s="3"/>
       <c r="Q19" s="3"/>
     </row>
-    <row r="20" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1">
+    <row r="20" spans="1:17" s="1" customFormat="1" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G20" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="H20" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
@@ -2394,27 +2402,27 @@
       <c r="P20" s="3"/>
       <c r="Q20" s="3"/>
     </row>
-    <row r="21" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1">
+    <row r="21" spans="1:17" s="1" customFormat="1" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>245</v>
-      </c>
       <c r="E21" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G21" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="H21" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
@@ -2422,100 +2430,100 @@
       <c r="P21" s="3"/>
       <c r="Q21" s="3"/>
     </row>
-    <row r="22" spans="1:17" ht="30">
+    <row r="22" spans="1:17" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" ht="30">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="3" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G23" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="H23" s="2" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" ht="30">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="3" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G24" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="H24" s="2" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" ht="30">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="3" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G25" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="H25" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -2533,71 +2541,71 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38:J38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.33203125" customWidth="1"/>
     <col min="2" max="2" width="8" customWidth="1"/>
-    <col min="3" max="3" width="21.83203125" customWidth="1"/>
-    <col min="4" max="4" width="14.5" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" customWidth="1"/>
-    <col min="6" max="6" width="15.5" customWidth="1"/>
-    <col min="7" max="7" width="30.83203125" customWidth="1"/>
-    <col min="8" max="8" width="27.83203125" customWidth="1"/>
-    <col min="9" max="9" width="12.5" customWidth="1"/>
+    <col min="3" max="3" width="21.77734375" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" customWidth="1"/>
+    <col min="7" max="7" width="30.77734375" customWidth="1"/>
+    <col min="8" max="8" width="27.77734375" customWidth="1"/>
+    <col min="9" max="9" width="12.44140625" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
-    <col min="11" max="11" width="16.83203125" customWidth="1"/>
+    <col min="11" max="11" width="16.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="45" customFormat="1" ht="30">
+    <row r="1" spans="1:15" s="45" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A1" s="44" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D1" s="45" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F1" s="45" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G1" s="45" t="s">
-        <v>2</v>
+        <v>316</v>
       </c>
       <c r="H1" s="45" t="s">
-        <v>7</v>
+        <v>315</v>
       </c>
       <c r="I1" s="45" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J1" s="45" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="K1" s="44" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="L1" s="44"/>
       <c r="M1" s="44"/>
       <c r="N1" s="44"/>
       <c r="O1" s="44"/>
     </row>
-    <row r="2" spans="1:15" s="1" customFormat="1">
+    <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
@@ -2605,19 +2613,19 @@
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
     </row>
-    <row r="3" spans="1:15" s="1" customFormat="1" ht="90">
+    <row r="3" spans="1:15" s="1" customFormat="1" ht="94.25" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="D3" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -2625,13 +2633,13 @@
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
     </row>
-    <row r="4" spans="1:15" s="10" customFormat="1" ht="30">
+    <row r="4" spans="1:15" s="10" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A4" s="9"/>
       <c r="B4" s="10" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="K4" s="9"/>
       <c r="L4" s="9"/>
@@ -2639,19 +2647,19 @@
       <c r="N4" s="9"/>
       <c r="O4" s="9"/>
     </row>
-    <row r="5" spans="1:15" s="10" customFormat="1" ht="30">
+    <row r="5" spans="1:15" s="10" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A5" s="9"/>
       <c r="D5" s="10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
@@ -2659,16 +2667,16 @@
       <c r="N5" s="9"/>
       <c r="O5" s="9"/>
     </row>
-    <row r="6" spans="1:15" s="10" customFormat="1" ht="75">
+    <row r="6" spans="1:15" s="10" customFormat="1" ht="78.55" x14ac:dyDescent="0.3">
       <c r="A6" s="9"/>
       <c r="D6" s="10" t="s">
         <v>1</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="I6" s="50" t="b">
         <v>1</v>
@@ -2677,17 +2685,17 @@
         <v>1</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
       <c r="N6" s="9"/>
       <c r="O6" s="9"/>
     </row>
-    <row r="7" spans="1:15" s="10" customFormat="1">
+    <row r="7" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9"/>
       <c r="B7" s="10" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
@@ -2695,19 +2703,19 @@
       <c r="N7" s="9"/>
       <c r="O7" s="9"/>
     </row>
-    <row r="8" spans="1:15" s="10" customFormat="1" ht="30">
+    <row r="8" spans="1:15" s="10" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A8" s="9"/>
       <c r="D8" s="10" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
@@ -2715,10 +2723,10 @@
       <c r="N8" s="9"/>
       <c r="O8" s="9"/>
     </row>
-    <row r="9" spans="1:15" s="10" customFormat="1">
+    <row r="9" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9"/>
       <c r="B9" s="10" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="K9" s="9"/>
       <c r="L9" s="9"/>
@@ -2726,19 +2734,19 @@
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
     </row>
-    <row r="10" spans="1:15" s="1" customFormat="1" ht="45">
+    <row r="10" spans="1:15" s="1" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="D10" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
@@ -2746,13 +2754,13 @@
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
     </row>
-    <row r="11" spans="1:15" s="12" customFormat="1" ht="30">
+    <row r="11" spans="1:15" s="12" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A11" s="11"/>
       <c r="B11" s="12" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="K11" s="11"/>
       <c r="L11" s="11"/>
@@ -2760,19 +2768,19 @@
       <c r="N11" s="11"/>
       <c r="O11" s="11"/>
     </row>
-    <row r="12" spans="1:15" s="12" customFormat="1" ht="30">
+    <row r="12" spans="1:15" s="12" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
       <c r="D12" s="12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="K12" s="11"/>
       <c r="L12" s="11"/>
@@ -2780,16 +2788,16 @@
       <c r="N12" s="11"/>
       <c r="O12" s="11"/>
     </row>
-    <row r="13" spans="1:15" s="12" customFormat="1" ht="75">
+    <row r="13" spans="1:15" s="12" customFormat="1" ht="78.55" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
       <c r="D13" s="12" t="s">
         <v>1</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="I13" s="51" t="b">
         <v>1</v>
@@ -2798,17 +2806,17 @@
         <v>1</v>
       </c>
       <c r="K13" s="11" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="L13" s="11"/>
       <c r="M13" s="11"/>
       <c r="N13" s="11"/>
       <c r="O13" s="11"/>
     </row>
-    <row r="14" spans="1:15" s="12" customFormat="1">
+    <row r="14" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11"/>
       <c r="B14" s="12" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="K14" s="11"/>
       <c r="L14" s="11"/>
@@ -2816,7 +2824,7 @@
       <c r="N14" s="11"/>
       <c r="O14" s="11"/>
     </row>
-    <row r="15" spans="1:15" s="28" customFormat="1">
+    <row r="15" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="27"/>
       <c r="K15" s="27"/>
       <c r="L15" s="27"/>
@@ -2824,13 +2832,13 @@
       <c r="N15" s="27"/>
       <c r="O15" s="27"/>
     </row>
-    <row r="16" spans="1:15" s="1" customFormat="1">
+    <row r="16" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="D16" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
@@ -2838,19 +2846,19 @@
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
     </row>
-    <row r="17" spans="1:15" s="1" customFormat="1" ht="60">
+    <row r="17" spans="1:15" s="1" customFormat="1" ht="62.85" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="D17" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
@@ -2858,13 +2866,13 @@
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
     </row>
-    <row r="18" spans="1:15" s="26" customFormat="1" ht="30">
+    <row r="18" spans="1:15" s="26" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A18" s="16"/>
       <c r="B18" s="26" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="K18" s="16"/>
       <c r="L18" s="16"/>
@@ -2872,19 +2880,19 @@
       <c r="N18" s="16"/>
       <c r="O18" s="16"/>
     </row>
-    <row r="19" spans="1:15" s="26" customFormat="1" ht="30">
+    <row r="19" spans="1:15" s="26" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A19" s="16"/>
       <c r="D19" s="26" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E19" s="26" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F19" s="26" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="G19" s="26" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="K19" s="16"/>
       <c r="L19" s="16"/>
@@ -2892,19 +2900,19 @@
       <c r="N19" s="16"/>
       <c r="O19" s="16"/>
     </row>
-    <row r="20" spans="1:15" s="26" customFormat="1" ht="30">
+    <row r="20" spans="1:15" s="26" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A20" s="16"/>
       <c r="D20" s="26" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E20" s="26" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F20" s="26" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="G20" s="26" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="K20" s="16"/>
       <c r="L20" s="16"/>
@@ -2912,13 +2920,13 @@
       <c r="N20" s="16"/>
       <c r="O20" s="16"/>
     </row>
-    <row r="21" spans="1:15" s="10" customFormat="1" ht="30">
+    <row r="21" spans="1:15" s="10" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A21" s="9"/>
       <c r="B21" s="10" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="K21" s="9"/>
       <c r="L21" s="9"/>
@@ -2926,19 +2934,19 @@
       <c r="N21" s="9"/>
       <c r="O21" s="9"/>
     </row>
-    <row r="22" spans="1:15" s="10" customFormat="1">
+    <row r="22" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="9"/>
       <c r="D22" s="10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="K22" s="9"/>
       <c r="L22" s="9"/>
@@ -2946,13 +2954,13 @@
       <c r="N22" s="9"/>
       <c r="O22" s="9"/>
     </row>
-    <row r="23" spans="1:15" s="8" customFormat="1" ht="30">
+    <row r="23" spans="1:15" s="8" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
       <c r="B23" s="8" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="K23" s="7"/>
       <c r="L23" s="7"/>
@@ -2960,16 +2968,16 @@
       <c r="N23" s="7"/>
       <c r="O23" s="7"/>
     </row>
-    <row r="24" spans="1:15" s="8" customFormat="1">
+    <row r="24" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="7"/>
       <c r="D24" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="K24" s="7"/>
       <c r="L24" s="7"/>
@@ -2977,10 +2985,10 @@
       <c r="N24" s="7"/>
       <c r="O24" s="7"/>
     </row>
-    <row r="25" spans="1:15" s="8" customFormat="1">
+    <row r="25" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7"/>
       <c r="B25" s="8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="K25" s="7"/>
       <c r="L25" s="7"/>
@@ -2988,10 +2996,10 @@
       <c r="N25" s="7"/>
       <c r="O25" s="7"/>
     </row>
-    <row r="26" spans="1:15" s="10" customFormat="1">
+    <row r="26" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9"/>
       <c r="B26" s="10" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="K26" s="9"/>
       <c r="L26" s="9"/>
@@ -2999,10 +3007,10 @@
       <c r="N26" s="9"/>
       <c r="O26" s="9"/>
     </row>
-    <row r="27" spans="1:15" s="26" customFormat="1">
+    <row r="27" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="16"/>
       <c r="B27" s="26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="K27" s="16"/>
       <c r="L27" s="16"/>
@@ -3010,7 +3018,7 @@
       <c r="N27" s="16"/>
       <c r="O27" s="16"/>
     </row>
-    <row r="28" spans="1:15" s="1" customFormat="1">
+    <row r="28" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
@@ -3018,32 +3026,32 @@
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
     </row>
-    <row r="29" spans="1:15" s="1" customFormat="1">
+    <row r="29" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="D29" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
     </row>
-    <row r="30" spans="1:15" s="1" customFormat="1" ht="60">
+    <row r="30" spans="1:15" s="1" customFormat="1" ht="62.85" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="D30" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
@@ -3051,13 +3059,13 @@
       <c r="N30" s="3"/>
       <c r="O30" s="3"/>
     </row>
-    <row r="31" spans="1:15" s="12" customFormat="1" ht="30">
+    <row r="31" spans="1:15" s="12" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A31" s="11"/>
       <c r="B31" s="12" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="K31" s="11"/>
       <c r="L31" s="11"/>
@@ -3065,16 +3073,16 @@
       <c r="N31" s="11"/>
       <c r="O31" s="11"/>
     </row>
-    <row r="32" spans="1:15" s="12" customFormat="1">
+    <row r="32" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="11"/>
       <c r="D32" s="12" t="s">
         <v>1</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G32" s="12" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I32" s="51" t="b">
         <v>1</v>
@@ -3083,10 +3091,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:15" s="12" customFormat="1">
+    <row r="33" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="11"/>
       <c r="B33" s="12" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="K33" s="11"/>
       <c r="L33" s="11"/>
@@ -3094,21 +3102,21 @@
       <c r="N33" s="11"/>
       <c r="O33" s="11"/>
     </row>
-    <row r="34" spans="1:15" s="30" customFormat="1" ht="45">
+    <row r="34" spans="1:15" s="30" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
       <c r="A34" s="29" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D34" s="30" t="s">
         <v>1</v>
       </c>
       <c r="E34" s="30" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="G34" s="30" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H34" s="30" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="I34" s="52" t="b">
         <v>1</v>
@@ -3117,13 +3125,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:15" s="1" customFormat="1">
+    <row r="35" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
       <c r="D35" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
@@ -3131,15 +3139,15 @@
       <c r="N35" s="3"/>
       <c r="O35" s="3"/>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D36" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="I36" t="b">
         <v>1</v>
@@ -3148,23 +3156,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D37" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D38" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="I38" t="b">
         <v>1</v>
@@ -3188,45 +3196,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.5" customWidth="1"/>
-    <col min="3" max="3" width="33.83203125" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" customWidth="1"/>
+    <col min="3" max="3" width="33.77734375" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" customWidth="1"/>
-    <col min="6" max="6" width="21.5" customWidth="1"/>
+    <col min="6" max="6" width="21.44140625" customWidth="1"/>
     <col min="7" max="7" width="38.6640625" customWidth="1"/>
     <col min="8" max="8" width="54" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="45" customFormat="1">
+    <row r="1" spans="1:13" s="45" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="44" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D1" s="45" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F1" s="45" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G1" s="45" t="s">
-        <v>2</v>
+        <v>316</v>
       </c>
       <c r="H1" s="45" t="s">
-        <v>7</v>
+        <v>315</v>
       </c>
       <c r="I1" s="44"/>
       <c r="J1" s="44"/>
@@ -3234,16 +3242,16 @@
       <c r="L1" s="44"/>
       <c r="M1" s="44"/>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" ht="105">
+    <row r="2" spans="1:13" s="1" customFormat="1" ht="105.4" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -3251,21 +3259,21 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" ht="30">
+    <row r="3" spans="1:13" s="1" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
@@ -3273,12 +3281,12 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:13" s="32" customFormat="1" ht="45">
+    <row r="4" spans="1:13" s="32" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
       <c r="A4" s="31" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
@@ -3291,21 +3299,21 @@
       <c r="L4" s="31"/>
       <c r="M4" s="31"/>
     </row>
-    <row r="5" spans="1:13" s="32" customFormat="1" ht="30">
+    <row r="5" spans="1:13" s="32" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A5" s="31" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B5" s="31"/>
       <c r="C5" s="31"/>
       <c r="D5" s="31" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E5" s="31"/>
       <c r="F5" s="31" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G5" s="31" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I5" s="31"/>
       <c r="J5" s="31"/>
@@ -3313,13 +3321,13 @@
       <c r="L5" s="31"/>
       <c r="M5" s="31"/>
     </row>
-    <row r="6" spans="1:13" s="10" customFormat="1" ht="30">
+    <row r="6" spans="1:13" s="10" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A6" s="9"/>
       <c r="B6" s="9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
@@ -3331,21 +3339,21 @@
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
     </row>
-    <row r="7" spans="1:13" s="10" customFormat="1">
+    <row r="7" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
@@ -3353,10 +3361,10 @@
       <c r="L7" s="9"/>
       <c r="M7" s="9"/>
     </row>
-    <row r="8" spans="1:13" s="10" customFormat="1">
+    <row r="8" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9"/>
       <c r="B8" s="9" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
@@ -3369,10 +3377,10 @@
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
     </row>
-    <row r="9" spans="1:13" s="32" customFormat="1">
+    <row r="9" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="31"/>
       <c r="B9" s="31" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C9" s="31"/>
       <c r="D9" s="31"/>
@@ -3385,21 +3393,21 @@
       <c r="L9" s="31"/>
       <c r="M9" s="31"/>
     </row>
-    <row r="10" spans="1:13" s="1" customFormat="1" ht="30">
+    <row r="10" spans="1:13" s="1" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
@@ -3407,10 +3415,10 @@
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
     </row>
-    <row r="11" spans="1:13" s="25" customFormat="1" ht="30">
+    <row r="11" spans="1:13" s="25" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A11" s="17"/>
       <c r="B11" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C11" s="17"/>
       <c r="D11" s="17"/>
@@ -3423,21 +3431,21 @@
       <c r="L11" s="17"/>
       <c r="M11" s="17"/>
     </row>
-    <row r="12" spans="1:13" s="25" customFormat="1" ht="30">
+    <row r="12" spans="1:13" s="25" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A12" s="17"/>
       <c r="B12" s="17"/>
       <c r="C12" s="17"/>
       <c r="D12" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="F12" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>36</v>
-      </c>
       <c r="G12" s="17" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I12" s="17"/>
       <c r="J12" s="17"/>
@@ -3445,13 +3453,13 @@
       <c r="L12" s="17"/>
       <c r="M12" s="17"/>
     </row>
-    <row r="13" spans="1:13" s="10" customFormat="1">
+    <row r="13" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9"/>
       <c r="B13" s="9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
@@ -3463,21 +3471,21 @@
       <c r="L13" s="9"/>
       <c r="M13" s="9"/>
     </row>
-    <row r="14" spans="1:13" s="10" customFormat="1" ht="30">
+    <row r="14" spans="1:13" s="10" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
       <c r="D14" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
@@ -3485,10 +3493,10 @@
       <c r="L14" s="9"/>
       <c r="M14" s="9"/>
     </row>
-    <row r="15" spans="1:13" s="10" customFormat="1">
+    <row r="15" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9"/>
       <c r="B15" s="9" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
@@ -3501,10 +3509,10 @@
       <c r="L15" s="9"/>
       <c r="M15" s="9"/>
     </row>
-    <row r="16" spans="1:13" s="25" customFormat="1">
+    <row r="16" spans="1:13" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="17"/>
       <c r="B16" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
@@ -3517,21 +3525,21 @@
       <c r="L16" s="17"/>
       <c r="M16" s="17"/>
     </row>
-    <row r="17" spans="1:13" s="1" customFormat="1" ht="30">
+    <row r="17" spans="1:13" s="1" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
@@ -3539,13 +3547,13 @@
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
     </row>
-    <row r="18" spans="1:13" s="12" customFormat="1" ht="30">
+    <row r="18" spans="1:13" s="12" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A18" s="11"/>
       <c r="B18" s="11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
@@ -3557,21 +3565,21 @@
       <c r="L18" s="11"/>
       <c r="M18" s="11"/>
     </row>
-    <row r="19" spans="1:13" s="12" customFormat="1" ht="30">
+    <row r="19" spans="1:13" s="12" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
       <c r="D19" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E19" s="11"/>
       <c r="F19" s="11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="I19" s="11"/>
       <c r="J19" s="11"/>
@@ -3579,10 +3587,10 @@
       <c r="L19" s="11"/>
       <c r="M19" s="11"/>
     </row>
-    <row r="20" spans="1:13" s="12" customFormat="1">
+    <row r="20" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="11"/>
       <c r="B20" s="11" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
@@ -3595,21 +3603,21 @@
       <c r="L20" s="11"/>
       <c r="M20" s="11"/>
     </row>
-    <row r="21" spans="1:13" s="1" customFormat="1" ht="30">
+    <row r="21" spans="1:13" s="1" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
@@ -3617,21 +3625,21 @@
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
     </row>
-    <row r="22" spans="1:13" s="1" customFormat="1" ht="30">
+    <row r="22" spans="1:13" s="1" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
@@ -3655,45 +3663,45 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.83203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="19.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.77734375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="29.33203125" style="1" customWidth="1"/>
-    <col min="4" max="6" width="14.5" style="1" customWidth="1"/>
+    <col min="4" max="6" width="14.44140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="34" style="1" customWidth="1"/>
     <col min="8" max="8" width="32.33203125" style="1" customWidth="1"/>
-    <col min="9" max="13" width="10.83203125" style="3"/>
-    <col min="14" max="16384" width="10.83203125" style="1"/>
+    <col min="9" max="13" width="10.77734375" style="3"/>
+    <col min="14" max="16384" width="10.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="45" customFormat="1">
+    <row r="1" spans="1:13" s="45" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="44" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D1" s="45" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F1" s="45" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G1" s="45" t="s">
-        <v>2</v>
+        <v>316</v>
       </c>
       <c r="H1" s="45" t="s">
-        <v>7</v>
+        <v>315</v>
       </c>
       <c r="I1" s="44"/>
       <c r="J1" s="44"/>
@@ -3701,26 +3709,26 @@
       <c r="L1" s="44"/>
       <c r="M1" s="44"/>
     </row>
-    <row r="2" spans="1:13" ht="45">
+    <row r="2" spans="1:13" ht="47.15" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" s="6" customFormat="1" ht="60">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" s="6" customFormat="1" ht="62.85" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
@@ -3728,10 +3736,10 @@
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
     </row>
-    <row r="7" spans="1:13" s="6" customFormat="1">
+    <row r="7" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
       <c r="B7" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
@@ -3739,10 +3747,10 @@
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
     </row>
-    <row r="9" spans="1:13" s="6" customFormat="1">
+    <row r="9" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="6" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
@@ -3750,10 +3758,10 @@
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
     </row>
-    <row r="11" spans="1:13" s="6" customFormat="1">
+    <row r="11" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
@@ -3761,10 +3769,10 @@
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
     </row>
-    <row r="13" spans="1:13" s="6" customFormat="1">
+    <row r="13" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="6" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
@@ -3772,10 +3780,10 @@
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
     </row>
-    <row r="15" spans="1:13" s="6" customFormat="1">
+    <row r="15" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -3783,10 +3791,10 @@
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
     </row>
-    <row r="17" spans="1:13" s="6" customFormat="1">
+    <row r="17" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="6" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
@@ -3813,275 +3821,275 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.5" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" customWidth="1"/>
-    <col min="3" max="3" width="26.5" customWidth="1"/>
+    <col min="3" max="3" width="26.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="46" customFormat="1">
+    <row r="1" spans="1:3" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B1" s="46" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C1" s="46" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="37" customFormat="1">
+    <row r="2" spans="1:3" s="37" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="37" t="s">
-        <v>113</v>
-      </c>
-      <c r="C2" s="37" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" s="37" customFormat="1">
+    </row>
+    <row r="3" spans="1:3" s="37" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="37" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C3" s="37" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" s="38" customFormat="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="38" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B4" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="38" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="C4" s="16" t="s">
+    </row>
+    <row r="6" spans="1:3" s="39" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" s="38" customFormat="1">
-      <c r="A5" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="B5" s="16" t="s">
+      <c r="C6" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C5" s="16" t="s">
+    </row>
+    <row r="7" spans="1:3" s="39" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" s="39" customFormat="1">
-      <c r="A6" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="B6" s="7" t="s">
+      <c r="C7" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C6" s="7" t="s">
+    </row>
+    <row r="8" spans="1:3" s="39" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" s="39" customFormat="1">
-      <c r="A7" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="B7" s="7" t="s">
+      <c r="C8" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" s="39" customFormat="1">
-      <c r="A8" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" s="40" customFormat="1">
+    </row>
+    <row r="9" spans="1:3" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="C10" s="9" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C12" s="9" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="40" customFormat="1">
-      <c r="A10" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="B10" s="9" t="s">
+    <row r="13" spans="1:3" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C13" s="9" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="40" customFormat="1">
-      <c r="A11" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="B11" s="9" t="s">
+    <row r="14" spans="1:3" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="B14" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C14" s="9" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="40" customFormat="1">
-      <c r="A12" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="B12" s="9" t="s">
+    <row r="15" spans="1:3" s="40" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="B15" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C15" s="9" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="40" customFormat="1">
-      <c r="A13" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" s="40" customFormat="1">
-      <c r="A14" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>226</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" s="40" customFormat="1" ht="30">
-      <c r="A15" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>227</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" s="41" customFormat="1">
+    <row r="16" spans="1:3" s="41" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B16" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="41" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="C17" s="11" t="s">
         <v>256</v>
       </c>
-      <c r="C16" s="11" t="s">
+    </row>
+    <row r="18" spans="1:3" s="42" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" s="42" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="B19" s="13" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" s="41" customFormat="1">
-      <c r="A17" s="11" t="s">
-        <v>251</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C17" s="11" t="s">
+      <c r="C19" s="13" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" s="42" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="B20" s="13" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" s="42" customFormat="1">
-      <c r="A18" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>260</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" s="42" customFormat="1">
-      <c r="A19" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>261</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" s="42" customFormat="1">
-      <c r="A20" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="B20" s="13" t="s">
+      <c r="C20" s="13" t="s">
         <v>262</v>
       </c>
-      <c r="C20" s="13" t="s">
+    </row>
+    <row r="21" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="17" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" s="43" customFormat="1">
-      <c r="A21" s="17" t="s">
+      <c r="B21" s="17" t="s">
+        <v>267</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="B22" s="17" t="s">
         <v>268</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="C22" s="17" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>269</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" s="43" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
+      <c r="A24" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="B24" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C24" s="17" t="s">
         <v>274</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" s="43" customFormat="1">
-      <c r="A22" s="17" t="s">
-        <v>268</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>271</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" s="43" customFormat="1">
-      <c r="A23" s="17" t="s">
-        <v>268</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>272</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" s="43" customFormat="1" ht="30">
-      <c r="A24" s="17" t="s">
-        <v>268</v>
-      </c>
-      <c r="B24" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -4100,139 +4108,139 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19" style="3" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" style="3" customWidth="1"/>
     <col min="3" max="3" width="21.33203125" style="3" customWidth="1"/>
     <col min="4" max="4" width="36" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="3"/>
+    <col min="5" max="16384" width="10.77734375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="44" customFormat="1">
+    <row r="1" spans="1:4" s="44" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="C1" s="44" t="s">
+        <v>317</v>
+      </c>
+      <c r="D1" s="44" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="B2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="48"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="D1" s="44" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="48"/>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="B3" s="3">
         <v>20131025</v>
       </c>
       <c r="D3" s="48"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="48"/>
+    </row>
+    <row r="5" spans="1:4" ht="31.45" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="48"/>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="D5" s="48"/>
     </row>
-    <row r="6" spans="1:4" ht="30">
+    <row r="6" spans="1:4" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D6" s="48" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D7" s="48"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D8" s="48"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="D6" s="48" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="D9" s="48"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="D7" s="48"/>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="D10" s="48"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="D8" s="48"/>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="D9" s="48"/>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="D11" s="48"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="D10" s="48"/>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="D11" s="48"/>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>180</v>
-      </c>
       <c r="D12" s="48"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D13" s="48"/>
     </row>
@@ -4252,46 +4260,46 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.1640625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="39.109375" style="3" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="15.77734375" style="3" customWidth="1"/>
     <col min="4" max="4" width="21" style="3" customWidth="1"/>
     <col min="5" max="5" width="32.6640625" style="3" customWidth="1"/>
     <col min="6" max="6" width="24.33203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="23.5" style="3" customWidth="1"/>
-    <col min="8" max="8" width="24.5" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="3"/>
+    <col min="7" max="7" width="29.33203125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="24.44140625" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="10.77734375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="45" customFormat="1">
+    <row r="1" spans="1:13" s="45" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="44" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B1" s="45" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D1" s="45" t="s">
-        <v>2</v>
+        <v>316</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>7</v>
+        <v>315</v>
       </c>
       <c r="F1" s="45" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G1" s="45" t="s">
-        <v>56</v>
+        <v>318</v>
       </c>
       <c r="H1" s="45" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="I1" s="44"/>
       <c r="J1" s="44"/>
@@ -4299,7 +4307,7 @@
       <c r="L1" s="44"/>
       <c r="M1" s="44"/>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" ht="33" customHeight="1">
+    <row r="2" spans="1:13" s="1" customFormat="1" ht="33.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -4308,31 +4316,31 @@
         <v>6</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" ht="76" customHeight="1">
+    <row r="3" spans="1:13" s="1" customFormat="1" ht="75.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="G3" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
@@ -4340,15 +4348,15 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:13" s="1" customFormat="1" ht="109" customHeight="1">
+    <row r="4" spans="1:13" s="1" customFormat="1" ht="109" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>4</v>
@@ -4381,47 +4389,47 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="3"/>
-    <col min="2" max="2" width="12.5" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="3"/>
-    <col min="4" max="4" width="24.5" style="3" customWidth="1"/>
-    <col min="5" max="5" width="23.5" style="3" customWidth="1"/>
+    <col min="1" max="1" width="10.77734375" style="3"/>
+    <col min="2" max="2" width="12.44140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" style="3"/>
+    <col min="4" max="4" width="24.44140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="23.44140625" style="3" customWidth="1"/>
     <col min="6" max="6" width="29.6640625" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="3"/>
+    <col min="7" max="16384" width="10.77734375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="44" customFormat="1">
+    <row r="1" spans="1:14" s="44" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="44" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B1" s="44" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="44" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D1" s="44" t="s">
-        <v>2</v>
+        <v>316</v>
       </c>
       <c r="E1" s="44" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F1" s="44" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" ht="30" customHeight="1">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="1" customFormat="1" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="3"/>
@@ -4430,16 +4438,16 @@
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:14" s="1" customFormat="1" ht="30" customHeight="1">
+    <row r="3" spans="1:14" s="1" customFormat="1" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E3" s="49" t="b">
         <v>1</v>
@@ -4452,7 +4460,7 @@
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:14" s="1" customFormat="1">
+    <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="C4" s="3"/>
       <c r="G4" s="3"/>
@@ -4476,54 +4484,54 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.1640625" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="1" max="1" width="24.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="18.33203125" customWidth="1"/>
-    <col min="5" max="5" width="31.1640625" customWidth="1"/>
-    <col min="6" max="6" width="23.1640625" customWidth="1"/>
-    <col min="7" max="7" width="25.83203125" customWidth="1"/>
+    <col min="5" max="5" width="31.109375" customWidth="1"/>
+    <col min="6" max="6" width="23.109375" customWidth="1"/>
+    <col min="7" max="7" width="25.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="46" customFormat="1">
+    <row r="1" spans="1:12" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="44" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B1" s="44" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="44" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D1" s="44" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E1" s="44" t="s">
-        <v>2</v>
+        <v>316</v>
       </c>
       <c r="F1" s="44" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G1" s="44" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="H1" s="44"/>
       <c r="I1" s="44"/>
       <c r="J1" s="44"/>
       <c r="K1" s="44"/>
     </row>
-    <row r="2" spans="1:12" s="1" customFormat="1">
+    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -4531,17 +4539,17 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:12" ht="30">
+    <row r="3" spans="1:12" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F3" s="49" t="b">
         <v>1</v>
@@ -4554,128 +4562,128 @@
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:12" s="3" customFormat="1" ht="90">
+    <row r="4" spans="1:12" s="3" customFormat="1" ht="94.25" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="3" customFormat="1" ht="45">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="3" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" s="3" customFormat="1" ht="45">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="3" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" s="3" customFormat="1" ht="30">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="3" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" s="3" customFormat="1" ht="30">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="3" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="3" customFormat="1" ht="45">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="3" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" s="3" customFormat="1" ht="45">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="3" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" s="3" customFormat="1" ht="30">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="3" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -4688,7 +4696,7 @@
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -4701,7 +4709,7 @@
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -4714,7 +4722,7 @@
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -4727,7 +4735,7 @@
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -4740,7 +4748,7 @@
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -4753,7 +4761,7 @@
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -4766,7 +4774,7 @@
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -4779,7 +4787,7 @@
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -4792,7 +4800,7 @@
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -4805,7 +4813,7 @@
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -4818,7 +4826,7 @@
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -4831,7 +4839,7 @@
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -4844,7 +4852,7 @@
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -4873,66 +4881,66 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="37.6640625" style="3" customWidth="1"/>
     <col min="2" max="2" width="8.33203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="33.83203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="3"/>
+    <col min="3" max="3" width="33.77734375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="10.77734375" style="3"/>
     <col min="6" max="6" width="14.6640625" style="3" customWidth="1"/>
     <col min="7" max="7" width="28.6640625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" customWidth="1"/>
-    <col min="10" max="10" width="28.5" style="3" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="3"/>
+    <col min="8" max="8" width="23.88671875" customWidth="1"/>
+    <col min="9" max="9" width="24.6640625" customWidth="1"/>
+    <col min="10" max="10" width="28.44140625" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="10.77734375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="45" customFormat="1" ht="30">
+    <row r="1" spans="1:13" s="45" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A1" s="44" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D1" s="45" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F1" s="45" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G1" s="45" t="s">
-        <v>2</v>
+        <v>316</v>
       </c>
       <c r="H1" s="44" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I1" s="44" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="J1" s="44" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="K1" s="44"/>
       <c r="L1" s="44"/>
       <c r="M1" s="44"/>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" ht="30">
+    <row r="2" spans="1:13" s="1" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -4940,32 +4948,32 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" ht="30">
+    <row r="3" spans="1:13" s="1" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:13" s="8" customFormat="1">
+    <row r="4" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
       <c r="B4" s="7" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
@@ -4976,21 +4984,21 @@
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
     </row>
-    <row r="5" spans="1:13" s="8" customFormat="1">
+    <row r="5" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
@@ -4999,10 +5007,10 @@
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
     </row>
-    <row r="6" spans="1:13" s="8" customFormat="1">
+    <row r="6" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
       <c r="B6" s="8" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
@@ -5015,19 +5023,19 @@
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
     </row>
-    <row r="7" spans="1:13" s="8" customFormat="1" ht="60">
+    <row r="7" spans="1:13" s="8" customFormat="1" ht="62.85" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="D7" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
@@ -5036,13 +5044,13 @@
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
     </row>
-    <row r="8" spans="1:13" s="10" customFormat="1">
+    <row r="8" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9"/>
       <c r="B8" s="10" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
@@ -5055,19 +5063,19 @@
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
     </row>
-    <row r="9" spans="1:13" s="10" customFormat="1">
+    <row r="9" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9"/>
       <c r="D9" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
@@ -5076,10 +5084,10 @@
       <c r="L9" s="9"/>
       <c r="M9" s="9"/>
     </row>
-    <row r="10" spans="1:13" s="10" customFormat="1">
+    <row r="10" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9"/>
       <c r="B10" s="10" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
@@ -5092,10 +5100,10 @@
       <c r="L10" s="9"/>
       <c r="M10" s="9"/>
     </row>
-    <row r="11" spans="1:13" s="8" customFormat="1">
+    <row r="11" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
       <c r="B11" s="8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -5108,13 +5116,13 @@
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
     </row>
-    <row r="12" spans="1:13" s="14" customFormat="1">
+    <row r="12" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13"/>
       <c r="B12" s="14" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
@@ -5123,18 +5131,18 @@
       <c r="L12" s="13"/>
       <c r="M12" s="13"/>
     </row>
-    <row r="13" spans="1:13" s="14" customFormat="1" ht="90">
+    <row r="13" spans="1:13" s="14" customFormat="1" ht="94.25" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>1</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="H13" s="53" t="b">
         <v>1</v>
@@ -5143,16 +5151,16 @@
         <v>1</v>
       </c>
       <c r="J13" s="15" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
       <c r="M13" s="13"/>
     </row>
-    <row r="14" spans="1:13" s="14" customFormat="1">
+    <row r="14" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="13"/>
       <c r="B14" s="14" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H14" s="13"/>
       <c r="I14" s="13"/>
@@ -5161,43 +5169,43 @@
       <c r="L14" s="13"/>
       <c r="M14" s="13"/>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="8:9">
+    <row r="17" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="8:9">
+    <row r="18" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="8:9">
+    <row r="19" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="8:9">
+    <row r="20" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
     </row>
-    <row r="21" spans="8:9">
+    <row r="21" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="8:9">
+    <row r="22" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="8:9">
+    <row r="23" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
     </row>
-    <row r="24" spans="8:9">
+    <row r="24" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
     </row>
@@ -5216,64 +5224,64 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView topLeftCell="F15" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25:J25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G1:G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.83203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="3"/>
-    <col min="3" max="3" width="29.1640625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="15.1640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="3"/>
+    <col min="1" max="1" width="29.77734375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" style="3"/>
+    <col min="3" max="3" width="29.109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="10.77734375" style="3"/>
     <col min="6" max="6" width="25.33203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="35.83203125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="25.5" style="3" customWidth="1"/>
-    <col min="9" max="10" width="10.83203125" style="3"/>
+    <col min="7" max="7" width="35.77734375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="25.44140625" style="3" customWidth="1"/>
+    <col min="9" max="10" width="23.88671875" style="3" customWidth="1"/>
     <col min="11" max="11" width="21.6640625" style="3" customWidth="1"/>
-    <col min="12" max="16384" width="10.83203125" style="3"/>
+    <col min="12" max="16384" width="10.77734375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="45" customFormat="1" ht="45">
+    <row r="1" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="44" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D1" s="45" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F1" s="45" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G1" s="45" t="s">
-        <v>2</v>
+        <v>316</v>
       </c>
       <c r="H1" s="45" t="s">
-        <v>7</v>
+        <v>315</v>
       </c>
       <c r="I1" s="44" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J1" s="44" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="K1" s="44" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="L1" s="44"/>
       <c r="M1" s="44"/>
       <c r="N1" s="44"/>
     </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" ht="90">
+    <row r="2" spans="1:14" s="1" customFormat="1" ht="94.25" x14ac:dyDescent="0.3">
       <c r="A2" s="18"/>
       <c r="B2" s="19"/>
       <c r="C2" s="19"/>
@@ -5283,10 +5291,10 @@
       <c r="E2" s="19"/>
       <c r="F2" s="19"/>
       <c r="G2" s="19" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="H2" s="19" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="I2" s="18"/>
       <c r="J2" s="18"/>
@@ -5294,36 +5302,36 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:14" ht="45">
+    <row r="3" spans="1:14" ht="47.15" x14ac:dyDescent="0.3">
       <c r="A3" s="18"/>
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
       <c r="D3" s="18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
       <c r="J3" s="18"/>
       <c r="K3" s="18"/>
     </row>
-    <row r="4" spans="1:14" s="16" customFormat="1" ht="90">
+    <row r="4" spans="1:14" s="16" customFormat="1" ht="94.25" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D4" s="20"/>
       <c r="E4" s="20"/>
@@ -5334,7 +5342,7 @@
       <c r="J4" s="20"/>
       <c r="K4" s="20"/>
     </row>
-    <row r="5" spans="1:14" s="16" customFormat="1" ht="45">
+    <row r="5" spans="1:14" s="16" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
       <c r="B5" s="20"/>
       <c r="C5" s="20"/>
@@ -5342,11 +5350,11 @@
         <v>1</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F5" s="20"/>
       <c r="G5" s="20" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="H5" s="20"/>
       <c r="I5" s="20" t="b">
@@ -5356,37 +5364,37 @@
         <v>1</v>
       </c>
       <c r="K5" s="20" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" s="16" customFormat="1" ht="30">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" s="16" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A6" s="20"/>
       <c r="B6" s="20"/>
       <c r="C6" s="20"/>
       <c r="D6" s="20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="H6" s="20"/>
       <c r="I6" s="20"/>
       <c r="J6" s="20"/>
       <c r="K6" s="20"/>
     </row>
-    <row r="7" spans="1:14" s="17" customFormat="1">
+    <row r="7" spans="1:14" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="21"/>
       <c r="B7" s="21" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D7" s="21"/>
       <c r="E7" s="21"/>
@@ -5397,31 +5405,31 @@
       <c r="J7" s="21"/>
       <c r="K7" s="21"/>
     </row>
-    <row r="8" spans="1:14" s="17" customFormat="1" ht="30">
+    <row r="8" spans="1:14" s="17" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A8" s="21"/>
       <c r="B8" s="21"/>
       <c r="C8" s="21"/>
       <c r="D8" s="21" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E8" s="21"/>
       <c r="F8" s="21" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="G8" s="21" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="H8" s="21" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="I8" s="21"/>
       <c r="J8" s="21"/>
       <c r="K8" s="21"/>
     </row>
-    <row r="9" spans="1:14" s="17" customFormat="1">
+    <row r="9" spans="1:14" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="21"/>
       <c r="B9" s="21" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C9" s="21"/>
       <c r="D9" s="21"/>
@@ -5433,10 +5441,10 @@
       <c r="J9" s="21"/>
       <c r="K9" s="21"/>
     </row>
-    <row r="10" spans="1:14" s="16" customFormat="1">
+    <row r="10" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="20"/>
       <c r="B10" s="20" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C10" s="20"/>
       <c r="D10" s="20"/>
@@ -5448,34 +5456,34 @@
       <c r="J10" s="20"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="1:14" ht="30">
+    <row r="11" spans="1:14" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
       <c r="B11" s="18"/>
       <c r="C11" s="18"/>
       <c r="D11" s="18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="H11" s="18"/>
       <c r="I11" s="18"/>
       <c r="J11" s="18"/>
       <c r="K11" s="18"/>
     </row>
-    <row r="12" spans="1:14" s="9" customFormat="1" ht="45">
+    <row r="12" spans="1:14" s="9" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
       <c r="A12" s="22"/>
       <c r="B12" s="22" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D12" s="22"/>
       <c r="E12" s="22"/>
@@ -5486,7 +5494,7 @@
       <c r="J12" s="22"/>
       <c r="K12" s="22"/>
     </row>
-    <row r="13" spans="1:14" s="9" customFormat="1" ht="45">
+    <row r="13" spans="1:14" s="9" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
       <c r="A13" s="22"/>
       <c r="B13" s="22"/>
       <c r="C13" s="22"/>
@@ -5494,11 +5502,11 @@
         <v>1</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F13" s="22"/>
       <c r="G13" s="22" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="H13" s="22"/>
       <c r="I13" s="22" t="b">
@@ -5508,13 +5516,13 @@
         <v>1</v>
       </c>
       <c r="K13" s="22" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" s="9" customFormat="1">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="22"/>
       <c r="B14" s="22" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
@@ -5526,34 +5534,34 @@
       <c r="J14" s="22"/>
       <c r="K14" s="22"/>
     </row>
-    <row r="15" spans="1:14" ht="30">
+    <row r="15" spans="1:14" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A15" s="18"/>
       <c r="B15" s="18"/>
       <c r="C15" s="18"/>
       <c r="D15" s="18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F15" s="18" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G15" s="18" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="H15" s="18"/>
       <c r="I15" s="18"/>
       <c r="J15" s="18"/>
       <c r="K15" s="18"/>
     </row>
-    <row r="16" spans="1:14" s="11" customFormat="1" ht="60">
+    <row r="16" spans="1:14" s="11" customFormat="1" ht="62.85" x14ac:dyDescent="0.3">
       <c r="A16" s="23"/>
       <c r="B16" s="23" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D16" s="23"/>
       <c r="E16" s="23"/>
@@ -5564,7 +5572,7 @@
       <c r="J16" s="23"/>
       <c r="K16" s="23"/>
     </row>
-    <row r="17" spans="1:11" s="11" customFormat="1" ht="45">
+    <row r="17" spans="1:11" s="11" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
       <c r="A17" s="23"/>
       <c r="B17" s="23"/>
       <c r="C17" s="23"/>
@@ -5572,11 +5580,11 @@
         <v>1</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="23" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="H17" s="23"/>
       <c r="I17" s="23" t="b">
@@ -5586,13 +5594,13 @@
         <v>1</v>
       </c>
       <c r="K17" s="23" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" s="11" customFormat="1">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="23"/>
       <c r="B18" s="23" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C18" s="23"/>
       <c r="D18" s="23"/>
@@ -5604,34 +5612,34 @@
       <c r="J18" s="23"/>
       <c r="K18" s="23"/>
     </row>
-    <row r="19" spans="1:11" ht="30">
+    <row r="19" spans="1:11" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A19" s="18"/>
       <c r="B19" s="18"/>
       <c r="C19" s="18"/>
       <c r="D19" s="18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F19" s="18" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="G19" s="18" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H19" s="18"/>
       <c r="I19" s="18"/>
       <c r="J19" s="18"/>
       <c r="K19" s="18"/>
     </row>
-    <row r="20" spans="1:11" s="5" customFormat="1" ht="45">
+    <row r="20" spans="1:11" s="5" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
       <c r="A20" s="24"/>
       <c r="B20" s="24" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D20" s="24"/>
       <c r="E20" s="24"/>
@@ -5642,7 +5650,7 @@
       <c r="J20" s="24"/>
       <c r="K20" s="24"/>
     </row>
-    <row r="21" spans="1:11" s="5" customFormat="1" ht="45">
+    <row r="21" spans="1:11" s="5" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
       <c r="A21" s="24"/>
       <c r="B21" s="24"/>
       <c r="C21" s="24"/>
@@ -5650,11 +5658,11 @@
         <v>1</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F21" s="24"/>
       <c r="G21" s="24" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="H21" s="24"/>
       <c r="I21" s="24" t="b">
@@ -5664,13 +5672,13 @@
         <v>1</v>
       </c>
       <c r="K21" s="24" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" s="5" customFormat="1">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="24"/>
       <c r="B22" s="24" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C22" s="24"/>
       <c r="D22" s="24"/>
@@ -5682,34 +5690,34 @@
       <c r="J22" s="24"/>
       <c r="K22" s="24"/>
     </row>
-    <row r="23" spans="1:11" ht="30">
+    <row r="23" spans="1:11" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A23" s="18"/>
       <c r="B23" s="18"/>
       <c r="C23" s="18"/>
       <c r="D23" s="18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F23" s="18" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="G23" s="18" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="H23" s="18"/>
       <c r="I23" s="18"/>
       <c r="J23" s="18"/>
       <c r="K23" s="18"/>
     </row>
-    <row r="24" spans="1:11" s="17" customFormat="1" ht="60">
+    <row r="24" spans="1:11" s="17" customFormat="1" ht="62.85" x14ac:dyDescent="0.3">
       <c r="A24" s="21"/>
       <c r="B24" s="21" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="D24" s="21"/>
       <c r="E24" s="21"/>
@@ -5720,7 +5728,7 @@
       <c r="J24" s="21"/>
       <c r="K24" s="21"/>
     </row>
-    <row r="25" spans="1:11" s="17" customFormat="1" ht="45">
+    <row r="25" spans="1:11" s="17" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
       <c r="A25" s="21"/>
       <c r="B25" s="21"/>
       <c r="C25" s="21"/>
@@ -5728,11 +5736,11 @@
         <v>1</v>
       </c>
       <c r="E25" s="21" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F25" s="21"/>
       <c r="G25" s="21" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="H25" s="21"/>
       <c r="I25" s="21" t="b">
@@ -5742,13 +5750,13 @@
         <v>1</v>
       </c>
       <c r="K25" s="21" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" s="17" customFormat="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="21"/>
       <c r="B26" s="21" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C26" s="21"/>
       <c r="D26" s="21"/>
@@ -5760,7 +5768,7 @@
       <c r="J26" s="21"/>
       <c r="K26" s="21"/>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="18"/>
       <c r="B27" s="18"/>
       <c r="C27" s="18"/>
@@ -5770,16 +5778,16 @@
       <c r="E27" s="18"/>
       <c r="F27" s="18"/>
       <c r="G27" s="18" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="H27" s="18"/>
       <c r="I27" s="18"/>
       <c r="J27" s="18"/>
       <c r="K27" s="18"/>
     </row>
-    <row r="28" spans="1:11" s="29" customFormat="1">
+    <row r="28" spans="1:11" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="47" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B28" s="47"/>
       <c r="C28" s="47"/>

</xml_diff>

<commit_message>
Partial check-in during mind-numbing edit. push survey Uri construction into Java side so it is implemented just once.  Add odkCommon.closeWindow API.
</commit_message>
<xml_diff>
--- a/app/config/tables/Ethiopia_household/forms/Ethiopia_household/Ethiopia_household.xlsx
+++ b/app/config/tables/Ethiopia_household/forms/Ethiopia_household/Ethiopia_household.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="65" yWindow="0" windowWidth="30737" windowHeight="16665" tabRatio="500" activeTab="10"/>
+    <workbookView xWindow="65" yWindow="0" windowWidth="30737" windowHeight="16665" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="queries" sheetId="9" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="321">
   <si>
     <t>type</t>
   </si>
@@ -108,9 +108,6 @@
     <t>[ data('household_id') ]</t>
   </si>
   <si>
-    <t>auxillaryHash</t>
-  </si>
-  <si>
     <t>Ethiopia_household</t>
   </si>
   <si>
@@ -978,9 +975,6 @@
     <t>filters by both the household_id and the age</t>
   </si>
   <si>
-    <t>'household_id='+opendatakit.encodeURIDataElement('household_id')</t>
-  </si>
-  <si>
     <t>display.hint.text</t>
   </si>
   <si>
@@ -991,6 +985,18 @@
   </si>
   <si>
     <t>display.new_instance_label.text</t>
+  </si>
+  <si>
+    <t>newRowInitialElementKeyToValueMap</t>
+  </si>
+  <si>
+    <t>openRowInitialElementKeyToValueMap</t>
+  </si>
+  <si>
+    <t>{ household_id : data('household_id') }</t>
+  </si>
+  <si>
+    <t>{}</t>
   </si>
 </sst>
 </file>
@@ -1947,10 +1953,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q25"/>
+  <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView topLeftCell="C8" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -1963,23 +1969,24 @@
     <col min="6" max="6" width="23.33203125" customWidth="1"/>
     <col min="7" max="7" width="26.109375" customWidth="1"/>
     <col min="8" max="8" width="39.6640625" customWidth="1"/>
+    <col min="9" max="9" width="34.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="44" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B1" s="44" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="44" t="s">
         <v>102</v>
-      </c>
-      <c r="C1" s="44" t="s">
-        <v>103</v>
       </c>
       <c r="D1" s="45" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F1" s="45" t="s">
         <v>20</v>
@@ -1988,12 +1995,15 @@
         <v>22</v>
       </c>
       <c r="H1" s="45" t="s">
-        <v>24</v>
+        <v>317</v>
+      </c>
+      <c r="I1" s="46" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="36" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B2" s="33"/>
       <c r="C2" s="33"/>
@@ -2005,7 +2015,7 @@
     </row>
     <row r="3" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="36" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B3" s="33"/>
       <c r="C3" s="33"/>
@@ -2017,7 +2027,7 @@
     </row>
     <row r="4" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="36" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B4" s="33"/>
       <c r="C4" s="33"/>
@@ -2029,7 +2039,7 @@
     </row>
     <row r="5" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="36" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B5" s="33"/>
       <c r="C5" s="33"/>
@@ -2041,7 +2051,7 @@
     </row>
     <row r="6" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="36" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="33"/>
@@ -2053,7 +2063,7 @@
     </row>
     <row r="7" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="36" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B7" s="33"/>
       <c r="C7" s="33"/>
@@ -2075,19 +2085,19 @@
     </row>
     <row r="9" spans="1:17" ht="47.15" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>21</v>
@@ -2096,46 +2106,52 @@
         <v>23</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="31.45" x14ac:dyDescent="0.3">
+        <v>319</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" ht="31.45" x14ac:dyDescent="0.3">
+        <v>319</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>21</v>
@@ -2144,33 +2160,39 @@
         <v>23</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>314</v>
+        <v>319</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="12" spans="1:17" s="12" customFormat="1" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B12" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="C12" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>107</v>
-      </c>
       <c r="G12" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>314</v>
+        <v>319</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>320</v>
       </c>
       <c r="M12" s="11"/>
       <c r="N12" s="11"/>
@@ -2180,16 +2202,16 @@
     </row>
     <row r="13" spans="1:17" s="1" customFormat="1" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>21</v>
@@ -2198,7 +2220,10 @@
         <v>23</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>314</v>
+        <v>319</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>320</v>
       </c>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
@@ -2208,25 +2233,28 @@
     </row>
     <row r="14" spans="1:17" s="1" customFormat="1" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>132</v>
-      </c>
       <c r="E14" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>21</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>314</v>
+        <v>319</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>320</v>
       </c>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
@@ -2236,25 +2264,28 @@
     </row>
     <row r="15" spans="1:17" s="1" customFormat="1" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>139</v>
-      </c>
       <c r="E15" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>314</v>
+        <v>319</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>320</v>
       </c>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
@@ -2264,25 +2295,28 @@
     </row>
     <row r="16" spans="1:17" s="1" customFormat="1" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>151</v>
-      </c>
       <c r="E16" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>314</v>
+        <v>319</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>320</v>
       </c>
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
@@ -2292,25 +2326,28 @@
     </row>
     <row r="17" spans="1:17" s="1" customFormat="1" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>314</v>
+        <v>319</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>320</v>
       </c>
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
@@ -2320,25 +2357,28 @@
     </row>
     <row r="18" spans="1:17" s="1" customFormat="1" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>314</v>
+        <v>319</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>320</v>
       </c>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
@@ -2348,25 +2388,28 @@
     </row>
     <row r="19" spans="1:17" s="1" customFormat="1" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>314</v>
+        <v>319</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>320</v>
       </c>
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
@@ -2376,16 +2419,16 @@
     </row>
     <row r="20" spans="1:17" s="1" customFormat="1" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>21</v>
@@ -2394,7 +2437,10 @@
         <v>23</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>314</v>
+        <v>319</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>320</v>
       </c>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
@@ -2404,16 +2450,16 @@
     </row>
     <row r="21" spans="1:17" s="1" customFormat="1" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>21</v>
@@ -2422,7 +2468,10 @@
         <v>23</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>314</v>
+        <v>319</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>320</v>
       </c>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
@@ -2430,43 +2479,46 @@
       <c r="P21" s="3"/>
       <c r="Q21" s="3"/>
     </row>
-    <row r="22" spans="1:17" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>21</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" ht="31.45" x14ac:dyDescent="0.3">
+        <v>319</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>21</v>
@@ -2475,22 +2527,25 @@
         <v>23</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" ht="31.45" x14ac:dyDescent="0.3">
+        <v>319</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>21</v>
@@ -2499,22 +2554,25 @@
         <v>23</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" ht="31.45" x14ac:dyDescent="0.3">
+        <v>319</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>21</v>
@@ -2523,8 +2581,14 @@
         <v>23</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>314</v>
-      </c>
+        <v>319</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="1048576" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I1048576" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2562,37 +2626,37 @@
   <sheetData>
     <row r="1" spans="1:15" s="45" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A1" s="44" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D1" s="45" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F1" s="45" t="s">
         <v>17</v>
       </c>
       <c r="G1" s="45" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="H1" s="45" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I1" s="45" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J1" s="45" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K1" s="44" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L1" s="44"/>
       <c r="M1" s="44"/>
@@ -2605,7 +2669,7 @@
         <v>5</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
@@ -2616,16 +2680,16 @@
     <row r="3" spans="1:15" s="1" customFormat="1" ht="94.25" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="D3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>205</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>206</v>
       </c>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -2636,10 +2700,10 @@
     <row r="4" spans="1:15" s="10" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A4" s="9"/>
       <c r="B4" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K4" s="9"/>
       <c r="L4" s="9"/>
@@ -2650,16 +2714,16 @@
     <row r="5" spans="1:15" s="10" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A5" s="9"/>
       <c r="D5" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
@@ -2673,19 +2737,19 @@
         <v>1</v>
       </c>
       <c r="E6" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="G6" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="I6" s="50" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" s="50" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" s="9" t="s">
         <v>212</v>
-      </c>
-      <c r="I6" s="50" t="b">
-        <v>1</v>
-      </c>
-      <c r="J6" s="50" t="b">
-        <v>1</v>
-      </c>
-      <c r="K6" s="9" t="s">
-        <v>213</v>
       </c>
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
@@ -2695,7 +2759,7 @@
     <row r="7" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9"/>
       <c r="B7" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
@@ -2706,16 +2770,16 @@
     <row r="8" spans="1:15" s="10" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A8" s="9"/>
       <c r="D8" s="10" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E8" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="G8" s="10" t="s">
         <v>216</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>215</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>217</v>
       </c>
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
@@ -2726,7 +2790,7 @@
     <row r="9" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9"/>
       <c r="B9" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K9" s="9"/>
       <c r="L9" s="9"/>
@@ -2737,16 +2801,16 @@
     <row r="10" spans="1:15" s="1" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="D10" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
@@ -2757,10 +2821,10 @@
     <row r="11" spans="1:15" s="12" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A11" s="11"/>
       <c r="B11" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K11" s="11"/>
       <c r="L11" s="11"/>
@@ -2771,16 +2835,16 @@
     <row r="12" spans="1:15" s="12" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
       <c r="D12" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F12" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="G12" s="12" t="s">
         <v>237</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>238</v>
       </c>
       <c r="K12" s="11"/>
       <c r="L12" s="11"/>
@@ -2794,19 +2858,19 @@
         <v>1</v>
       </c>
       <c r="E13" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="G13" s="12" t="s">
         <v>239</v>
       </c>
-      <c r="G13" s="12" t="s">
+      <c r="I13" s="51" t="b">
+        <v>1</v>
+      </c>
+      <c r="J13" s="51" t="b">
+        <v>1</v>
+      </c>
+      <c r="K13" s="11" t="s">
         <v>240</v>
-      </c>
-      <c r="I13" s="51" t="b">
-        <v>1</v>
-      </c>
-      <c r="J13" s="51" t="b">
-        <v>1</v>
-      </c>
-      <c r="K13" s="11" t="s">
-        <v>241</v>
       </c>
       <c r="L13" s="11"/>
       <c r="M13" s="11"/>
@@ -2816,7 +2880,7 @@
     <row r="14" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11"/>
       <c r="B14" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K14" s="11"/>
       <c r="L14" s="11"/>
@@ -2838,7 +2902,7 @@
         <v>5</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
@@ -2849,16 +2913,16 @@
     <row r="17" spans="1:15" s="1" customFormat="1" ht="62.85" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="D17" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F17" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>244</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>245</v>
       </c>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
@@ -2869,10 +2933,10 @@
     <row r="18" spans="1:15" s="26" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A18" s="16"/>
       <c r="B18" s="26" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="K18" s="16"/>
       <c r="L18" s="16"/>
@@ -2883,16 +2947,16 @@
     <row r="19" spans="1:15" s="26" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A19" s="16"/>
       <c r="D19" s="26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E19" s="26" t="s">
+        <v>247</v>
+      </c>
+      <c r="F19" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="G19" s="26" t="s">
         <v>248</v>
-      </c>
-      <c r="F19" s="26" t="s">
-        <v>247</v>
-      </c>
-      <c r="G19" s="26" t="s">
-        <v>249</v>
       </c>
       <c r="K19" s="16"/>
       <c r="L19" s="16"/>
@@ -2903,16 +2967,16 @@
     <row r="20" spans="1:15" s="26" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A20" s="16"/>
       <c r="D20" s="26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E20" s="26" t="s">
+        <v>249</v>
+      </c>
+      <c r="F20" s="26" t="s">
         <v>250</v>
       </c>
-      <c r="F20" s="26" t="s">
+      <c r="G20" s="26" t="s">
         <v>251</v>
-      </c>
-      <c r="G20" s="26" t="s">
-        <v>252</v>
       </c>
       <c r="K20" s="16"/>
       <c r="L20" s="16"/>
@@ -2923,10 +2987,10 @@
     <row r="21" spans="1:15" s="10" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A21" s="9"/>
       <c r="B21" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="K21" s="9"/>
       <c r="L21" s="9"/>
@@ -2937,16 +3001,16 @@
     <row r="22" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="9"/>
       <c r="D22" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E22" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="F22" s="10" t="s">
         <v>265</v>
       </c>
-      <c r="F22" s="10" t="s">
-        <v>266</v>
-      </c>
       <c r="G22" s="10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K22" s="9"/>
       <c r="L22" s="9"/>
@@ -2957,10 +3021,10 @@
     <row r="23" spans="1:15" s="8" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
       <c r="B23" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="K23" s="7"/>
       <c r="L23" s="7"/>
@@ -2974,10 +3038,10 @@
         <v>16</v>
       </c>
       <c r="F24" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="G24" s="8" t="s">
         <v>276</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>277</v>
       </c>
       <c r="K24" s="7"/>
       <c r="L24" s="7"/>
@@ -2988,7 +3052,7 @@
     <row r="25" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7"/>
       <c r="B25" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K25" s="7"/>
       <c r="L25" s="7"/>
@@ -2999,7 +3063,7 @@
     <row r="26" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9"/>
       <c r="B26" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K26" s="9"/>
       <c r="L26" s="9"/>
@@ -3010,7 +3074,7 @@
     <row r="27" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="16"/>
       <c r="B27" s="26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K27" s="16"/>
       <c r="L27" s="16"/>
@@ -3032,7 +3096,7 @@
         <v>5</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
@@ -3042,16 +3106,16 @@
     <row r="30" spans="1:15" s="1" customFormat="1" ht="62.85" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="D30" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F30" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G30" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
@@ -3062,10 +3126,10 @@
     <row r="31" spans="1:15" s="12" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A31" s="11"/>
       <c r="B31" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K31" s="11"/>
       <c r="L31" s="11"/>
@@ -3079,10 +3143,10 @@
         <v>1</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G32" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I32" s="51" t="b">
         <v>1</v>
@@ -3094,7 +3158,7 @@
     <row r="33" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="11"/>
       <c r="B33" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K33" s="11"/>
       <c r="L33" s="11"/>
@@ -3104,19 +3168,19 @@
     </row>
     <row r="34" spans="1:15" s="30" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
       <c r="A34" s="29" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D34" s="30" t="s">
         <v>1</v>
       </c>
       <c r="E34" s="30" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G34" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="H34" s="30" t="s">
         <v>55</v>
-      </c>
-      <c r="H34" s="30" t="s">
-        <v>56</v>
       </c>
       <c r="I34" s="52" t="b">
         <v>1</v>
@@ -3131,7 +3195,7 @@
         <v>5</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
@@ -3144,10 +3208,10 @@
         <v>1</v>
       </c>
       <c r="E36" t="s">
+        <v>287</v>
+      </c>
+      <c r="G36" s="1" t="s">
         <v>288</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>289</v>
       </c>
       <c r="I36" t="b">
         <v>1</v>
@@ -3161,7 +3225,7 @@
         <v>5</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.3">
@@ -3169,10 +3233,10 @@
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I38" t="b">
         <v>1</v>
@@ -3196,7 +3260,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
@@ -3213,28 +3277,28 @@
   <sheetData>
     <row r="1" spans="1:13" s="45" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="44" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D1" s="45" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F1" s="45" t="s">
         <v>17</v>
       </c>
       <c r="G1" s="45" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="H1" s="45" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I1" s="44"/>
       <c r="J1" s="44"/>
@@ -3248,10 +3312,10 @@
         <v>5</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>69</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>70</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -3264,16 +3328,16 @@
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
@@ -3283,10 +3347,10 @@
     </row>
     <row r="4" spans="1:13" s="32" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
       <c r="A4" s="31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
@@ -3301,7 +3365,7 @@
     </row>
     <row r="5" spans="1:13" s="32" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A5" s="31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B5" s="31"/>
       <c r="C5" s="31"/>
@@ -3310,10 +3374,10 @@
       </c>
       <c r="E5" s="31"/>
       <c r="F5" s="31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G5" s="31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I5" s="31"/>
       <c r="J5" s="31"/>
@@ -3324,10 +3388,10 @@
     <row r="6" spans="1:13" s="10" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A6" s="9"/>
       <c r="B6" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
@@ -3344,16 +3408,16 @@
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
@@ -3364,7 +3428,7 @@
     <row r="8" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9"/>
       <c r="B8" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
@@ -3380,7 +3444,7 @@
     <row r="9" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="31"/>
       <c r="B9" s="31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9" s="31"/>
       <c r="D9" s="31"/>
@@ -3398,16 +3462,16 @@
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="G10" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
@@ -3418,7 +3482,7 @@
     <row r="11" spans="1:13" s="25" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A11" s="17"/>
       <c r="B11" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C11" s="17"/>
       <c r="D11" s="17"/>
@@ -3436,16 +3500,16 @@
       <c r="B12" s="17"/>
       <c r="C12" s="17"/>
       <c r="D12" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I12" s="17"/>
       <c r="J12" s="17"/>
@@ -3456,10 +3520,10 @@
     <row r="13" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9"/>
       <c r="B13" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
@@ -3476,16 +3540,16 @@
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
       <c r="D14" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E14" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" s="9" t="s">
         <v>81</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>82</v>
       </c>
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
@@ -3496,7 +3560,7 @@
     <row r="15" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9"/>
       <c r="B15" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
@@ -3512,7 +3576,7 @@
     <row r="16" spans="1:13" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="17"/>
       <c r="B16" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
@@ -3530,16 +3594,16 @@
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
@@ -3550,10 +3614,10 @@
     <row r="18" spans="1:13" s="12" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A18" s="11"/>
       <c r="B18" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
@@ -3567,7 +3631,7 @@
     </row>
     <row r="19" spans="1:13" s="12" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
@@ -3576,10 +3640,10 @@
       </c>
       <c r="E19" s="11"/>
       <c r="F19" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I19" s="11"/>
       <c r="J19" s="11"/>
@@ -3590,7 +3654,7 @@
     <row r="20" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="11"/>
       <c r="B20" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
@@ -3608,16 +3672,16 @@
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
@@ -3630,16 +3694,16 @@
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
@@ -3680,28 +3744,28 @@
   <sheetData>
     <row r="1" spans="1:13" s="45" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="44" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D1" s="45" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F1" s="45" t="s">
         <v>17</v>
       </c>
       <c r="G1" s="45" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="H1" s="45" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I1" s="44"/>
       <c r="J1" s="44"/>
@@ -3711,7 +3775,7 @@
     </row>
     <row r="2" spans="1:13" ht="47.15" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>16</v>
@@ -3725,10 +3789,10 @@
     </row>
     <row r="5" spans="1:13" s="6" customFormat="1" ht="62.85" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
@@ -3739,7 +3803,7 @@
     <row r="7" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
       <c r="B7" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
@@ -3750,7 +3814,7 @@
     <row r="9" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
@@ -3761,7 +3825,7 @@
     <row r="11" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
@@ -3772,7 +3836,7 @@
     <row r="13" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
@@ -3783,7 +3847,7 @@
     <row r="15" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -3794,7 +3858,7 @@
     <row r="17" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
@@ -3830,10 +3894,10 @@
   <sheetData>
     <row r="1" spans="1:3" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="46" t="s">
         <v>61</v>
-      </c>
-      <c r="B1" s="46" t="s">
-        <v>62</v>
       </c>
       <c r="C1" s="46" t="s">
         <v>2</v>
@@ -3841,255 +3905,255 @@
     </row>
     <row r="2" spans="1:3" s="37" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="37" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3" s="37" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="38" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B4" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>88</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="38" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B5" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" s="16" t="s">
         <v>90</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="39" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B6" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>92</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="39" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>94</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="39" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B8" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>96</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="40" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="16" spans="1:3" s="41" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="41" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="18" spans="1:3" s="42" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="13" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="42" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="42" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="13" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="17" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="24" spans="1:3" s="43" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A24" s="17" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -4128,10 +4192,10 @@
         <v>11</v>
       </c>
       <c r="C1" s="44" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D1" s="44" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -4139,7 +4203,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D2" s="48"/>
     </row>
@@ -4157,7 +4221,7 @@
         <v>14</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D4" s="48"/>
     </row>
@@ -4166,78 +4230,78 @@
         <v>15</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" s="48"/>
     </row>
     <row r="6" spans="1:4" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D6" s="48" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D7" s="48"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D8" s="48"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D9" s="48"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D10" s="48"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>174</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>175</v>
       </c>
       <c r="D11" s="48"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>176</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>177</v>
       </c>
       <c r="D12" s="48"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>18</v>
@@ -4278,28 +4342,28 @@
   <sheetData>
     <row r="1" spans="1:13" s="45" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="44" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B1" s="45" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D1" s="45" t="s">
+        <v>314</v>
+      </c>
+      <c r="E1" s="45" t="s">
+        <v>313</v>
+      </c>
+      <c r="F1" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="45" t="s">
         <v>316</v>
       </c>
-      <c r="E1" s="45" t="s">
-        <v>315</v>
-      </c>
-      <c r="F1" s="45" t="s">
-        <v>52</v>
-      </c>
-      <c r="G1" s="45" t="s">
-        <v>318</v>
-      </c>
       <c r="H1" s="45" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I1" s="44"/>
       <c r="J1" s="44"/>
@@ -4325,13 +4389,13 @@
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" ht="75.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>8</v>
@@ -4340,7 +4404,7 @@
         <v>9</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
@@ -4350,13 +4414,13 @@
     </row>
     <row r="4" spans="1:13" s="1" customFormat="1" ht="109" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>4</v>
@@ -4405,22 +4469,22 @@
   <sheetData>
     <row r="1" spans="1:14" s="44" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="44" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B1" s="44" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="44" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D1" s="44" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E1" s="44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F1" s="44" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="1" customFormat="1" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -4429,7 +4493,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="3"/>
@@ -4444,10 +4508,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E3" s="49" t="b">
         <v>1</v>
@@ -4500,25 +4564,25 @@
   <sheetData>
     <row r="1" spans="1:12" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="44" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B1" s="44" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="44" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D1" s="44" t="s">
         <v>17</v>
       </c>
       <c r="E1" s="44" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F1" s="44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G1" s="44" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H1" s="44"/>
       <c r="I1" s="44"/>
@@ -4531,7 +4595,7 @@
         <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -4545,11 +4609,11 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F3" s="49" t="b">
         <v>1</v>
@@ -4564,123 +4628,123 @@
     </row>
     <row r="4" spans="1:12" s="3" customFormat="1" ht="94.25" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="3" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="3" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="7" spans="1:12" s="3" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:12" s="3" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="9" spans="1:12" s="3" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:12" s="3" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:12" s="3" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
@@ -4899,36 +4963,36 @@
     <col min="11" max="16384" width="10.77734375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="45" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="45" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="44" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D1" s="45" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F1" s="45" t="s">
         <v>17</v>
       </c>
       <c r="G1" s="45" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="H1" s="44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I1" s="44" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J1" s="44" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K1" s="44"/>
       <c r="L1" s="44"/>
@@ -4940,7 +5004,7 @@
         <v>5</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -4951,16 +5015,16 @@
     <row r="3" spans="1:13" s="1" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>113</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>114</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
@@ -4970,10 +5034,10 @@
     <row r="4" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
       <c r="B4" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
@@ -4989,16 +5053,16 @@
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E5" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>119</v>
-      </c>
       <c r="G5" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
@@ -5010,7 +5074,7 @@
     <row r="6" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
       <c r="B6" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
@@ -5026,16 +5090,16 @@
     <row r="7" spans="1:13" s="8" customFormat="1" ht="62.85" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="D7" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
@@ -5047,10 +5111,10 @@
     <row r="8" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9"/>
       <c r="B8" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
@@ -5066,16 +5130,16 @@
     <row r="9" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9"/>
       <c r="D9" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F9" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="G9" s="9" t="s">
         <v>124</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>125</v>
       </c>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
@@ -5087,7 +5151,7 @@
     <row r="10" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9"/>
       <c r="B10" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
@@ -5103,7 +5167,7 @@
     <row r="11" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
       <c r="B11" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -5119,10 +5183,10 @@
     <row r="12" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13"/>
       <c r="B12" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
@@ -5133,16 +5197,16 @@
     </row>
     <row r="13" spans="1:13" s="14" customFormat="1" ht="94.25" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>1</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H13" s="53" t="b">
         <v>1</v>
@@ -5151,7 +5215,7 @@
         <v>1</v>
       </c>
       <c r="J13" s="15" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
@@ -5160,7 +5224,7 @@
     <row r="14" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="13"/>
       <c r="B14" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H14" s="13"/>
       <c r="I14" s="13"/>
@@ -5245,37 +5309,37 @@
   <sheetData>
     <row r="1" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="44" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D1" s="45" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F1" s="45" t="s">
         <v>17</v>
       </c>
       <c r="G1" s="45" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="H1" s="45" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I1" s="44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J1" s="44" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K1" s="44" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L1" s="44"/>
       <c r="M1" s="44"/>
@@ -5291,10 +5355,10 @@
       <c r="E2" s="19"/>
       <c r="F2" s="19"/>
       <c r="G2" s="19" t="s">
+        <v>207</v>
+      </c>
+      <c r="H2" s="19" t="s">
         <v>208</v>
-      </c>
-      <c r="H2" s="19" t="s">
-        <v>209</v>
       </c>
       <c r="I2" s="18"/>
       <c r="J2" s="18"/>
@@ -5307,16 +5371,16 @@
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
       <c r="D3" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F3" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="G3" s="18" t="s">
         <v>136</v>
-      </c>
-      <c r="G3" s="18" t="s">
-        <v>137</v>
       </c>
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
@@ -5325,13 +5389,13 @@
     </row>
     <row r="4" spans="1:14" s="16" customFormat="1" ht="94.25" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D4" s="20"/>
       <c r="E4" s="20"/>
@@ -5350,11 +5414,11 @@
         <v>1</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F5" s="20"/>
       <c r="G5" s="20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H5" s="20"/>
       <c r="I5" s="20" t="b">
@@ -5364,7 +5428,7 @@
         <v>1</v>
       </c>
       <c r="K5" s="20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:14" s="16" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
@@ -5372,16 +5436,16 @@
       <c r="B6" s="20"/>
       <c r="C6" s="20"/>
       <c r="D6" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F6" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="G6" s="20" t="s">
         <v>141</v>
-      </c>
-      <c r="G6" s="20" t="s">
-        <v>142</v>
       </c>
       <c r="H6" s="20"/>
       <c r="I6" s="20"/>
@@ -5391,10 +5455,10 @@
     <row r="7" spans="1:14" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="21"/>
       <c r="B7" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D7" s="21"/>
       <c r="E7" s="21"/>
@@ -5410,17 +5474,17 @@
       <c r="B8" s="21"/>
       <c r="C8" s="21"/>
       <c r="D8" s="21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E8" s="21"/>
       <c r="F8" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="G8" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="G8" s="21" t="s">
+      <c r="H8" s="21" t="s">
         <v>146</v>
-      </c>
-      <c r="H8" s="21" t="s">
-        <v>147</v>
       </c>
       <c r="I8" s="21"/>
       <c r="J8" s="21"/>
@@ -5429,7 +5493,7 @@
     <row r="9" spans="1:14" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="21"/>
       <c r="B9" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C9" s="21"/>
       <c r="D9" s="21"/>
@@ -5444,7 +5508,7 @@
     <row r="10" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="20"/>
       <c r="B10" s="20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C10" s="20"/>
       <c r="D10" s="20"/>
@@ -5461,16 +5525,16 @@
       <c r="B11" s="18"/>
       <c r="C11" s="18"/>
       <c r="D11" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F11" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="G11" s="18" t="s">
         <v>148</v>
-      </c>
-      <c r="G11" s="18" t="s">
-        <v>149</v>
       </c>
       <c r="H11" s="18"/>
       <c r="I11" s="18"/>
@@ -5480,10 +5544,10 @@
     <row r="12" spans="1:14" s="9" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
       <c r="A12" s="22"/>
       <c r="B12" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D12" s="22"/>
       <c r="E12" s="22"/>
@@ -5502,11 +5566,11 @@
         <v>1</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F13" s="22"/>
       <c r="G13" s="22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H13" s="22"/>
       <c r="I13" s="22" t="b">
@@ -5516,13 +5580,13 @@
         <v>1</v>
       </c>
       <c r="K13" s="22" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="14" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="22"/>
       <c r="B14" s="22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
@@ -5539,16 +5603,16 @@
       <c r="B15" s="18"/>
       <c r="C15" s="18"/>
       <c r="D15" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F15" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="G15" s="18" t="s">
         <v>153</v>
-      </c>
-      <c r="G15" s="18" t="s">
-        <v>154</v>
       </c>
       <c r="H15" s="18"/>
       <c r="I15" s="18"/>
@@ -5558,10 +5622,10 @@
     <row r="16" spans="1:14" s="11" customFormat="1" ht="62.85" x14ac:dyDescent="0.3">
       <c r="A16" s="23"/>
       <c r="B16" s="23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D16" s="23"/>
       <c r="E16" s="23"/>
@@ -5580,11 +5644,11 @@
         <v>1</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H17" s="23"/>
       <c r="I17" s="23" t="b">
@@ -5594,13 +5658,13 @@
         <v>1</v>
       </c>
       <c r="K17" s="23" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="18" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="23"/>
       <c r="B18" s="23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C18" s="23"/>
       <c r="D18" s="23"/>
@@ -5617,16 +5681,16 @@
       <c r="B19" s="18"/>
       <c r="C19" s="18"/>
       <c r="D19" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F19" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="G19" s="18" t="s">
         <v>158</v>
-      </c>
-      <c r="G19" s="18" t="s">
-        <v>159</v>
       </c>
       <c r="H19" s="18"/>
       <c r="I19" s="18"/>
@@ -5636,10 +5700,10 @@
     <row r="20" spans="1:11" s="5" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
       <c r="A20" s="24"/>
       <c r="B20" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D20" s="24"/>
       <c r="E20" s="24"/>
@@ -5658,11 +5722,11 @@
         <v>1</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F21" s="24"/>
       <c r="G21" s="24" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H21" s="24"/>
       <c r="I21" s="24" t="b">
@@ -5672,13 +5736,13 @@
         <v>1</v>
       </c>
       <c r="K21" s="24" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="22" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="24"/>
       <c r="B22" s="24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C22" s="24"/>
       <c r="D22" s="24"/>
@@ -5695,16 +5759,16 @@
       <c r="B23" s="18"/>
       <c r="C23" s="18"/>
       <c r="D23" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F23" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="G23" s="18" t="s">
         <v>162</v>
-      </c>
-      <c r="G23" s="18" t="s">
-        <v>163</v>
       </c>
       <c r="H23" s="18"/>
       <c r="I23" s="18"/>
@@ -5714,10 +5778,10 @@
     <row r="24" spans="1:11" s="17" customFormat="1" ht="62.85" x14ac:dyDescent="0.3">
       <c r="A24" s="21"/>
       <c r="B24" s="21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D24" s="21"/>
       <c r="E24" s="21"/>
@@ -5736,11 +5800,11 @@
         <v>1</v>
       </c>
       <c r="E25" s="21" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F25" s="21"/>
       <c r="G25" s="21" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H25" s="21"/>
       <c r="I25" s="21" t="b">
@@ -5750,13 +5814,13 @@
         <v>1</v>
       </c>
       <c r="K25" s="21" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="26" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="21"/>
       <c r="B26" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C26" s="21"/>
       <c r="D26" s="21"/>
@@ -5778,7 +5842,7 @@
       <c r="E27" s="18"/>
       <c r="F27" s="18"/>
       <c r="G27" s="18" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H27" s="18"/>
       <c r="I27" s="18"/>
@@ -5787,7 +5851,7 @@
     </row>
     <row r="28" spans="1:11" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="47" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B28" s="47"/>
       <c r="C28" s="47"/>

</xml_diff>